<commit_message>
Dodanie obsługi tabeli typów wkładów elastomerowych. 	- Odczyt i zpapis typów do bazy danych. 	- Usunięcie typu z bazy danych. Aktualizacja wzorów kart dla łożysk garnkowych.
</commit_message>
<xml_diff>
--- a/data/wzor_PF.xlsx
+++ b/data/wzor_PF.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Arkusz1!$A$1:$R$56</definedName>
     <definedName name="Wybór1" localSheetId="0">Arkusz1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
   <si>
     <t>WYMIAR KONTROLNY</t>
   </si>
@@ -353,51 +353,6 @@
     <t>---</t>
   </si>
   <si>
-    <r>
-      <t>Luz między tłokiem a cylindrem 0.5&lt;(</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>t-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="7"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="238"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>D) ≤1</t>
-    </r>
-  </si>
-  <si>
     <t>POMIAR KONTROLNY</t>
   </si>
   <si>
@@ -540,6 +495,12 @@
   </si>
   <si>
     <t>F4.3.1 KARTA WYROBU – ŁOŻYSKO GARNKOWE zg. z PN EN 1337-5:2005</t>
+  </si>
+  <si>
+    <t>Luz między tłokiem a cylindrem 0.5&lt;(Dt-DD) ≤1</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -552,7 +513,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* \-??\ _z_ł_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;____######0_);[Red]\(&quot;$&quot;____#####0\)"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="41">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,6 +531,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
       <charset val="238"/>
     </font>
     <font>
@@ -774,20 +736,6 @@
       <charset val="238"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="7"/>
       <color theme="1"/>
       <name val="Tahoma"/>
@@ -830,6 +778,13 @@
       <b/>
       <sz val="9"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -891,7 +846,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -1354,6 +1309,145 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2460,7 +2554,7 @@
     <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2508,7 +2602,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2516,10 +2610,47 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2540,98 +2671,269 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2642,202 +2944,40 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -4045,7 +4185,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>102579</xdr:colOff>
+      <xdr:colOff>169815</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>138480</xdr:rowOff>
     </xdr:to>
@@ -4083,7 +4223,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>53045</xdr:colOff>
+      <xdr:colOff>109074</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>38832</xdr:rowOff>
     </xdr:to>
@@ -4121,7 +4261,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>104336</xdr:colOff>
+      <xdr:colOff>272424</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>146002</xdr:rowOff>
     </xdr:to>
@@ -4131,7 +4271,7 @@
         <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns="" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:ve="http://schemas.openxmlformats.org/markup-compatibility/2006" val="0"/>
@@ -4529,40 +4669,40 @@
   </sheetPr>
   <dimension ref="A2:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A28" zoomScale="130" zoomScaleNormal="70" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:R2"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="J16" zoomScale="130" zoomScaleNormal="70" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25:G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.19921875" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="7" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="18" width="4.59765625" customWidth="1"/>
-    <col min="19" max="19" width="4.296875" customWidth="1"/>
-    <col min="20" max="20" width="4.09765625" customWidth="1"/>
+    <col min="1" max="18" width="4.375" customWidth="1"/>
+    <col min="19" max="19" width="4.25" customWidth="1"/>
+    <col min="20" max="20" width="4.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A2" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="22"/>
+    <row r="2" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A2" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
+      <c r="M2" s="35"/>
+      <c r="N2" s="35"/>
+      <c r="O2" s="35"/>
+      <c r="P2" s="35"/>
+      <c r="Q2" s="35"/>
+      <c r="R2" s="35"/>
     </row>
-    <row r="3" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
+    <row r="3" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -4582,105 +4722,105 @@
       <c r="Q3" s="21"/>
       <c r="R3" s="21"/>
     </row>
-    <row r="4" spans="1:18" ht="13.2" customHeight="1" thickTop="1">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:18" ht="13.15" customHeight="1" thickTop="1">
+      <c r="A4" s="42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="43"/>
+      <c r="C4" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30" t="s">
+      <c r="D4" s="43"/>
+      <c r="E4" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30" t="s">
+      <c r="F4" s="43"/>
+      <c r="G4" s="43" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30" t="s">
+      <c r="H4" s="43"/>
+      <c r="I4" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30" t="s">
+      <c r="J4" s="43"/>
+      <c r="K4" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30" t="s">
+      <c r="L4" s="43"/>
+      <c r="M4" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30" t="s">
+      <c r="N4" s="43"/>
+      <c r="O4" s="43" t="s">
         <v>76</v>
       </c>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30" t="s">
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="R4" s="33"/>
+      <c r="R4" s="46"/>
     </row>
-    <row r="5" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A5" s="31"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32"/>
-      <c r="F5" s="32"/>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
-      <c r="L5" s="32"/>
-      <c r="M5" s="32"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
-      <c r="P5" s="32"/>
-      <c r="Q5" s="32"/>
-      <c r="R5" s="34"/>
+    <row r="5" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A5" s="44"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="45"/>
+      <c r="I5" s="45"/>
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="47"/>
     </row>
-    <row r="6" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A6" s="35"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="94"/>
-      <c r="N6" s="94"/>
-      <c r="O6" s="94"/>
-      <c r="P6" s="94"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="127"/>
+    <row r="6" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A6" s="48"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
+      <c r="K6" s="49"/>
+      <c r="L6" s="49"/>
+      <c r="M6" s="49"/>
+      <c r="N6" s="49"/>
+      <c r="O6" s="49"/>
+      <c r="P6" s="49"/>
+      <c r="Q6" s="49"/>
+      <c r="R6" s="108"/>
     </row>
-    <row r="7" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
-      <c r="A7" s="37"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="126"/>
-      <c r="N7" s="126"/>
-      <c r="O7" s="126"/>
-      <c r="P7" s="126"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="128"/>
+    <row r="7" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
+      <c r="A7" s="50"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+      <c r="E7" s="51"/>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="51"/>
+      <c r="M7" s="51"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
+      <c r="P7" s="51"/>
+      <c r="Q7" s="51"/>
+      <c r="R7" s="109"/>
     </row>
-    <row r="8" spans="1:18" ht="13.2" customHeight="1" thickTop="1">
+    <row r="8" spans="1:18" ht="13.15" customHeight="1" thickTop="1">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -4700,41 +4840,41 @@
       <c r="Q8" s="18"/>
       <c r="R8" s="18"/>
     </row>
-    <row r="9" spans="1:18" ht="13.2" customHeight="1">
+    <row r="9" spans="1:18" ht="13.15" customHeight="1">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="13.2" customHeight="1">
+    <row r="10" spans="1:18" ht="13.15" customHeight="1">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="13.2" customHeight="1">
+    <row r="11" spans="1:18" ht="13.15" customHeight="1">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="13.2" customHeight="1">
+    <row r="12" spans="1:18" ht="13.15" customHeight="1">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="13.2" customHeight="1">
+    <row r="13" spans="1:18" ht="13.15" customHeight="1">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="13.2" customHeight="1">
+    <row r="14" spans="1:18" ht="13.15" customHeight="1">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:18" ht="13.2" customHeight="1">
+    <row r="15" spans="1:18" ht="13.15" customHeight="1">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:18" ht="13.2" customHeight="1"/>
-    <row r="17" spans="1:18" ht="13.2" customHeight="1"/>
-    <row r="18" spans="1:18" ht="13.2" customHeight="1"/>
-    <row r="19" spans="1:18" ht="13.2" customHeight="1"/>
-    <row r="20" spans="1:18" s="5" customFormat="1" ht="13.2" customHeight="1">
+    <row r="16" spans="1:18" ht="13.15" customHeight="1"/>
+    <row r="17" spans="1:18" ht="13.15" customHeight="1"/>
+    <row r="18" spans="1:18" ht="13.15" customHeight="1"/>
+    <row r="19" spans="1:18" ht="13.15" customHeight="1"/>
+    <row r="20" spans="1:18" s="5" customFormat="1" ht="13.15" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="125"/>
-      <c r="H20" s="125"/>
-      <c r="I20" s="125"/>
+      <c r="G20" s="129"/>
+      <c r="H20" s="129"/>
+      <c r="I20" s="129"/>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
@@ -4745,7 +4885,7 @@
       <c r="Q20"/>
       <c r="R20"/>
     </row>
-    <row r="21" spans="1:18" s="5" customFormat="1" ht="13.2" customHeight="1">
+    <row r="21" spans="1:18" s="5" customFormat="1" ht="13.15" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="7"/>
@@ -4754,7 +4894,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="125"/>
+      <c r="I21" s="129"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
@@ -4765,7 +4905,7 @@
       <c r="Q21"/>
       <c r="R21"/>
     </row>
-    <row r="22" spans="1:18" s="5" customFormat="1" ht="13.2" customHeight="1">
+    <row r="22" spans="1:18" s="5" customFormat="1" ht="13.15" customHeight="1">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="8"/>
@@ -4776,13 +4916,13 @@
       <c r="H22" s="8"/>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
-      <c r="A23" s="93" t="s">
+    <row r="23" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
+      <c r="A23" s="98" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="93"/>
-      <c r="C23" s="93"/>
-      <c r="D23" s="101"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="98"/>
+      <c r="D23" s="107"/>
       <c r="E23" s="15" t="s">
         <v>8</v>
       </c>
@@ -4826,743 +4966,759 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A24" s="102" t="s">
+    <row r="24" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A24" s="110" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="102"/>
-      <c r="C24" s="102"/>
-      <c r="D24" s="103"/>
-      <c r="E24" s="16">
-        <v>380</v>
-      </c>
-      <c r="F24" s="12">
-        <v>380</v>
-      </c>
+      <c r="B24" s="110"/>
+      <c r="C24" s="110"/>
+      <c r="D24" s="111"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="12"/>
       <c r="G24" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="H24" s="13">
-        <v>380</v>
-      </c>
+      <c r="H24" s="13"/>
       <c r="I24" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J24" s="13">
-        <v>28</v>
-      </c>
-      <c r="K24" s="13">
-        <v>49</v>
-      </c>
-      <c r="L24" s="12">
-        <v>40</v>
-      </c>
-      <c r="M24" s="12">
-        <v>39</v>
-      </c>
-      <c r="N24" s="12">
-        <v>1</v>
-      </c>
-      <c r="O24" s="12">
-        <v>370</v>
-      </c>
-      <c r="P24" s="12">
-        <v>5</v>
-      </c>
-      <c r="Q24" s="12">
-        <v>2.8</v>
-      </c>
-      <c r="R24" s="12">
-        <v>123</v>
-      </c>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="M24" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="N24" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="O24" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="P24" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q24" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="R24" s="12"/>
     </row>
-    <row r="25" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A25" s="104" t="s">
+    <row r="25" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A25" s="112" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="105"/>
-      <c r="C25" s="105"/>
-      <c r="D25" s="106"/>
-      <c r="E25" s="110" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="110"/>
-      <c r="G25" s="111"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="113"/>
+      <c r="D25" s="114"/>
+      <c r="E25" s="138" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="138"/>
+      <c r="G25" s="139"/>
       <c r="H25" s="6">
         <v>0.5</v>
       </c>
-      <c r="I25" s="114" t="s">
+      <c r="I25" s="118" t="s">
         <v>22</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K25" s="115" t="s">
+      <c r="K25" s="119" t="s">
         <v>27</v>
       </c>
-      <c r="L25" s="117" t="s">
+      <c r="L25" s="121" t="s">
         <v>28</v>
       </c>
-      <c r="M25" s="118"/>
-      <c r="N25" s="119"/>
-      <c r="O25" s="123" t="s">
+      <c r="M25" s="122"/>
+      <c r="N25" s="123"/>
+      <c r="O25" s="127" t="s">
         <v>32</v>
       </c>
-      <c r="P25" s="96" t="s">
+      <c r="P25" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="Q25" s="96" t="s">
+      <c r="Q25" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="R25" s="97" t="s">
+      <c r="R25" s="103" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A26" s="107"/>
-      <c r="B26" s="108"/>
-      <c r="C26" s="108"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="112"/>
-      <c r="F26" s="112"/>
-      <c r="G26" s="113"/>
+    <row r="26" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A26" s="115"/>
+      <c r="B26" s="116"/>
+      <c r="C26" s="116"/>
+      <c r="D26" s="117"/>
+      <c r="E26" s="140"/>
+      <c r="F26" s="140"/>
+      <c r="G26" s="141"/>
       <c r="H26" s="3">
         <v>-1</v>
       </c>
-      <c r="I26" s="114"/>
+      <c r="I26" s="118"/>
       <c r="J26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K26" s="116"/>
-      <c r="L26" s="120"/>
-      <c r="M26" s="121"/>
-      <c r="N26" s="122"/>
-      <c r="O26" s="124"/>
-      <c r="P26" s="96"/>
-      <c r="Q26" s="96"/>
-      <c r="R26" s="97"/>
+      <c r="K26" s="120"/>
+      <c r="L26" s="124"/>
+      <c r="M26" s="125"/>
+      <c r="N26" s="126"/>
+      <c r="O26" s="128"/>
+      <c r="P26" s="102"/>
+      <c r="Q26" s="102"/>
+      <c r="R26" s="103"/>
     </row>
-    <row r="27" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A27" s="91" t="s">
+    <row r="27" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A27" s="96" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="98"/>
-      <c r="E27" s="99"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="100"/>
-      <c r="H27" s="100"/>
-      <c r="I27" s="100"/>
-      <c r="J27" s="50"/>
-      <c r="K27" s="50"/>
-      <c r="L27" s="50"/>
-      <c r="M27" s="50"/>
-      <c r="N27" s="50"/>
-      <c r="O27" s="50"/>
-      <c r="P27" s="50"/>
-      <c r="Q27" s="50"/>
-      <c r="R27" s="50"/>
+      <c r="B27" s="96"/>
+      <c r="C27" s="96"/>
+      <c r="D27" s="104"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="106"/>
+      <c r="G27" s="106"/>
+      <c r="H27" s="106"/>
+      <c r="I27" s="106"/>
+      <c r="J27" s="144"/>
+      <c r="K27" s="144"/>
+      <c r="L27" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="M27" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="N27" s="142" t="s">
+        <v>80</v>
+      </c>
+      <c r="O27" s="144" t="s">
+        <v>80</v>
+      </c>
+      <c r="P27" s="144" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q27" s="144" t="s">
+        <v>80</v>
+      </c>
+      <c r="R27" s="144"/>
     </row>
-    <row r="28" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A28" s="91"/>
-      <c r="B28" s="91"/>
-      <c r="C28" s="91"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="99"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="100"/>
-      <c r="H28" s="100"/>
-      <c r="I28" s="100"/>
-      <c r="J28" s="50"/>
-      <c r="K28" s="50"/>
-      <c r="L28" s="50"/>
-      <c r="M28" s="50"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="50"/>
-      <c r="P28" s="50"/>
-      <c r="Q28" s="50"/>
-      <c r="R28" s="50"/>
+    <row r="28" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A28" s="96"/>
+      <c r="B28" s="96"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="105"/>
+      <c r="F28" s="106"/>
+      <c r="G28" s="106"/>
+      <c r="H28" s="106"/>
+      <c r="I28" s="106"/>
+      <c r="J28" s="144"/>
+      <c r="K28" s="144"/>
+      <c r="L28" s="143"/>
+      <c r="M28" s="143"/>
+      <c r="N28" s="143"/>
+      <c r="O28" s="144"/>
+      <c r="P28" s="144"/>
+      <c r="Q28" s="144"/>
+      <c r="R28" s="144"/>
     </row>
-    <row r="29" spans="1:18" ht="13.2" customHeight="1"/>
-    <row r="30" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A30" s="91" t="s">
+    <row r="29" spans="1:18" ht="13.15" customHeight="1"/>
+    <row r="30" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A30" s="96" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="96"/>
+      <c r="C30" s="104"/>
+      <c r="D30" s="95" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="91"/>
-      <c r="C30" s="98"/>
-      <c r="D30" s="90" t="s">
+      <c r="E30" s="96"/>
+      <c r="F30" s="96"/>
+      <c r="G30" s="96"/>
+      <c r="H30" s="96"/>
+      <c r="I30" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="E30" s="91"/>
-      <c r="F30" s="91"/>
-      <c r="G30" s="91"/>
-      <c r="H30" s="91"/>
-      <c r="I30" s="91" t="s">
+      <c r="J30" s="96"/>
+      <c r="K30" s="96"/>
+      <c r="L30" s="96"/>
+      <c r="M30" s="96"/>
+      <c r="N30" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="J30" s="91"/>
-      <c r="K30" s="91"/>
-      <c r="L30" s="91"/>
-      <c r="M30" s="91"/>
-      <c r="N30" s="94" t="s">
+      <c r="O30" s="100"/>
+      <c r="P30" s="100"/>
+      <c r="Q30" s="100"/>
+      <c r="R30" s="100"/>
+    </row>
+    <row r="31" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A31" s="96"/>
+      <c r="B31" s="96"/>
+      <c r="C31" s="104"/>
+      <c r="D31" s="95"/>
+      <c r="E31" s="96"/>
+      <c r="F31" s="96"/>
+      <c r="G31" s="96"/>
+      <c r="H31" s="96"/>
+      <c r="I31" s="96"/>
+      <c r="J31" s="96"/>
+      <c r="K31" s="96"/>
+      <c r="L31" s="96"/>
+      <c r="M31" s="96"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="100"/>
+      <c r="P31" s="100"/>
+      <c r="Q31" s="100"/>
+      <c r="R31" s="100"/>
+    </row>
+    <row r="32" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
+      <c r="A32" s="98"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="107"/>
+      <c r="D32" s="97"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="98"/>
+      <c r="H32" s="98"/>
+      <c r="I32" s="98"/>
+      <c r="J32" s="98"/>
+      <c r="K32" s="98"/>
+      <c r="L32" s="98"/>
+      <c r="M32" s="98"/>
+      <c r="N32" s="101"/>
+      <c r="O32" s="101"/>
+      <c r="P32" s="101"/>
+      <c r="Q32" s="101"/>
+      <c r="R32" s="101"/>
+    </row>
+    <row r="33" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
+      <c r="A33" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="O30" s="36"/>
-      <c r="P30" s="36"/>
-      <c r="Q30" s="36"/>
-      <c r="R30" s="36"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="87" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="88"/>
+      <c r="F33" s="88"/>
+      <c r="G33" s="89"/>
+      <c r="H33" s="89"/>
+      <c r="I33" s="88" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" s="88"/>
+      <c r="K33" s="88"/>
+      <c r="L33" s="89"/>
+      <c r="M33" s="89"/>
+      <c r="N33" s="69" t="s">
+        <v>40</v>
+      </c>
+      <c r="O33" s="69"/>
+      <c r="P33" s="69"/>
+      <c r="Q33" s="70"/>
+      <c r="R33" s="70"/>
     </row>
-    <row r="31" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A31" s="91"/>
-      <c r="B31" s="91"/>
-      <c r="C31" s="98"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="91"/>
-      <c r="F31" s="91"/>
-      <c r="G31" s="91"/>
-      <c r="H31" s="91"/>
-      <c r="I31" s="91"/>
-      <c r="J31" s="91"/>
-      <c r="K31" s="91"/>
-      <c r="L31" s="91"/>
-      <c r="M31" s="91"/>
-      <c r="N31" s="36"/>
-      <c r="O31" s="36"/>
-      <c r="P31" s="36"/>
-      <c r="Q31" s="36"/>
-      <c r="R31" s="36"/>
+    <row r="34" spans="1:18" ht="13.15" customHeight="1">
+      <c r="A34" s="71" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="72"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" s="72"/>
+      <c r="F34" s="72"/>
+      <c r="G34" s="77"/>
+      <c r="H34" s="78"/>
+      <c r="I34" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="72"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="81"/>
+      <c r="M34" s="82"/>
+      <c r="N34" s="72" t="s">
+        <v>42</v>
+      </c>
+      <c r="O34" s="72"/>
+      <c r="P34" s="72"/>
+      <c r="Q34" s="81"/>
+      <c r="R34" s="82"/>
     </row>
-    <row r="32" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
-      <c r="A32" s="93"/>
-      <c r="B32" s="93"/>
-      <c r="C32" s="101"/>
-      <c r="D32" s="92"/>
-      <c r="E32" s="93"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="93"/>
-      <c r="H32" s="93"/>
-      <c r="I32" s="93"/>
-      <c r="J32" s="93"/>
-      <c r="K32" s="93"/>
-      <c r="L32" s="93"/>
-      <c r="M32" s="93"/>
-      <c r="N32" s="95"/>
-      <c r="O32" s="95"/>
-      <c r="P32" s="95"/>
-      <c r="Q32" s="95"/>
-      <c r="R32" s="95"/>
+    <row r="35" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
+      <c r="A35" s="74"/>
+      <c r="B35" s="75"/>
+      <c r="C35" s="76"/>
+      <c r="D35" s="75"/>
+      <c r="E35" s="75"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="79"/>
+      <c r="H35" s="80"/>
+      <c r="I35" s="75"/>
+      <c r="J35" s="75"/>
+      <c r="K35" s="75"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="84"/>
+      <c r="N35" s="75"/>
+      <c r="O35" s="75"/>
+      <c r="P35" s="75"/>
+      <c r="Q35" s="83"/>
+      <c r="R35" s="84"/>
     </row>
-    <row r="33" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
-      <c r="A33" s="83" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="83"/>
-      <c r="C33" s="84"/>
-      <c r="D33" s="85" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="86"/>
-      <c r="F33" s="86"/>
-      <c r="G33" s="87"/>
-      <c r="H33" s="87"/>
-      <c r="I33" s="86" t="s">
-        <v>40</v>
-      </c>
-      <c r="J33" s="86"/>
-      <c r="K33" s="86"/>
-      <c r="L33" s="87"/>
-      <c r="M33" s="87"/>
-      <c r="N33" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="O33" s="67"/>
-      <c r="P33" s="67"/>
-      <c r="Q33" s="68"/>
-      <c r="R33" s="68"/>
-    </row>
-    <row r="34" spans="1:18" ht="13.2" customHeight="1">
-      <c r="A34" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="70"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="75"/>
-      <c r="H34" s="76"/>
-      <c r="I34" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="79"/>
-      <c r="M34" s="80"/>
-      <c r="N34" s="70" t="s">
-        <v>43</v>
-      </c>
-      <c r="O34" s="70"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="79"/>
-      <c r="R34" s="80"/>
-    </row>
-    <row r="35" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
-      <c r="A35" s="72"/>
-      <c r="B35" s="73"/>
-      <c r="C35" s="74"/>
-      <c r="D35" s="73"/>
-      <c r="E35" s="73"/>
-      <c r="F35" s="73"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="78"/>
-      <c r="I35" s="73"/>
-      <c r="J35" s="73"/>
-      <c r="K35" s="73"/>
-      <c r="L35" s="81"/>
-      <c r="M35" s="82"/>
-      <c r="N35" s="73"/>
-      <c r="O35" s="73"/>
-      <c r="P35" s="73"/>
-      <c r="Q35" s="81"/>
-      <c r="R35" s="82"/>
-    </row>
-    <row r="37" spans="1:18" ht="14.4" thickBot="1">
-      <c r="B37" s="62" t="s">
+    <row r="37" spans="1:18" ht="15" thickBot="1">
+      <c r="A37" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="62"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="88"/>
-      <c r="F37" s="66" t="s">
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="91"/>
+      <c r="F37" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G37" s="62"/>
-      <c r="H37" s="62"/>
-      <c r="I37" s="62"/>
-      <c r="J37" s="62"/>
-      <c r="K37" s="62"/>
-      <c r="L37" s="62"/>
-      <c r="M37" s="62"/>
-      <c r="N37" s="62" t="s">
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="22"/>
+      <c r="N37" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="O37" s="62"/>
-      <c r="P37" s="62"/>
-      <c r="Q37" s="62"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="27"/>
+      <c r="R37" s="28"/>
     </row>
     <row r="38" spans="1:18">
-      <c r="B38" s="67" t="s">
+      <c r="A38" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="C38" s="67"/>
-      <c r="D38" s="67"/>
-      <c r="E38" s="89"/>
-      <c r="F38" s="64" t="s">
+      <c r="B38" s="68"/>
+      <c r="C38" s="68"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="93"/>
+      <c r="F38" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="64"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="64"/>
-      <c r="J38" s="64" t="s">
-        <v>57</v>
-      </c>
-      <c r="K38" s="64"/>
-      <c r="L38" s="64"/>
-      <c r="M38" s="65"/>
-      <c r="N38" s="63"/>
-      <c r="O38" s="63"/>
-      <c r="P38" s="63"/>
-      <c r="Q38" s="63"/>
+      <c r="G38" s="68"/>
+      <c r="H38" s="68"/>
+      <c r="I38" s="68"/>
+      <c r="J38" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="K38" s="68"/>
+      <c r="L38" s="68"/>
+      <c r="M38" s="68"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="30"/>
+      <c r="P38" s="30"/>
+      <c r="Q38" s="30"/>
+      <c r="R38" s="31"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="B39" s="60" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39" s="60"/>
-      <c r="D39" s="60"/>
-      <c r="E39" s="61"/>
-      <c r="F39" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="G39" s="51"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="51"/>
-      <c r="J39" s="51" t="s">
-        <v>58</v>
-      </c>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="50"/>
-      <c r="O39" s="50"/>
-      <c r="P39" s="50"/>
-      <c r="Q39" s="50"/>
+      <c r="A39" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="24"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" s="24"/>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24"/>
+      <c r="J39" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K39" s="24"/>
+      <c r="L39" s="24"/>
+      <c r="M39" s="24"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="34"/>
     </row>
     <row r="40" spans="1:18">
-      <c r="B40" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="C40" s="60"/>
-      <c r="D40" s="60"/>
-      <c r="E40" s="61"/>
-      <c r="F40" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="G40" s="51"/>
-      <c r="H40" s="51"/>
-      <c r="I40" s="51"/>
-      <c r="J40" s="51" t="s">
-        <v>59</v>
-      </c>
-      <c r="K40" s="51"/>
-      <c r="L40" s="51"/>
-      <c r="M40" s="52"/>
-      <c r="N40" s="50"/>
-      <c r="O40" s="50"/>
-      <c r="P40" s="50"/>
-      <c r="Q40" s="50"/>
+      <c r="A40" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
+      <c r="D40" s="24"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40" s="24"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K40" s="24"/>
+      <c r="L40" s="24"/>
+      <c r="M40" s="24"/>
+      <c r="N40" s="32"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="34"/>
     </row>
     <row r="41" spans="1:18">
-      <c r="B41" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41" s="60"/>
-      <c r="D41" s="60"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="51" t="s">
-        <v>52</v>
-      </c>
-      <c r="G41" s="51"/>
-      <c r="H41" s="51"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="K41" s="51"/>
-      <c r="L41" s="51"/>
-      <c r="M41" s="52"/>
-      <c r="N41" s="50"/>
-      <c r="O41" s="50"/>
-      <c r="P41" s="50"/>
-      <c r="Q41" s="50"/>
+      <c r="A41" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G41" s="24"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="61"/>
+      <c r="J41" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="K41" s="24"/>
+      <c r="L41" s="24"/>
+      <c r="M41" s="24"/>
+      <c r="N41" s="32"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="34"/>
     </row>
     <row r="42" spans="1:18">
-      <c r="B42" s="60" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="60"/>
-      <c r="D42" s="60"/>
-      <c r="E42" s="61"/>
-      <c r="F42" s="51" t="s">
-        <v>53</v>
-      </c>
-      <c r="G42" s="51"/>
-      <c r="H42" s="51"/>
-      <c r="I42" s="52"/>
-      <c r="J42" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="K42" s="51"/>
-      <c r="L42" s="51"/>
-      <c r="M42" s="52"/>
-      <c r="N42" s="50"/>
-      <c r="O42" s="50"/>
-      <c r="P42" s="50"/>
-      <c r="Q42" s="50"/>
+      <c r="A42" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B42" s="24"/>
+      <c r="C42" s="24"/>
+      <c r="D42" s="24"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="G42" s="24"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="61"/>
+      <c r="J42" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K42" s="24"/>
+      <c r="L42" s="24"/>
+      <c r="M42" s="24"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="33"/>
+      <c r="Q42" s="33"/>
+      <c r="R42" s="34"/>
     </row>
     <row r="43" spans="1:18">
-      <c r="B43" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="C43" s="60"/>
-      <c r="D43" s="60"/>
-      <c r="E43" s="61"/>
-      <c r="F43" s="51" t="s">
-        <v>54</v>
-      </c>
-      <c r="G43" s="51"/>
-      <c r="H43" s="51"/>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51" t="s">
-        <v>62</v>
-      </c>
-      <c r="K43" s="51"/>
-      <c r="L43" s="51"/>
-      <c r="M43" s="52"/>
-      <c r="N43" s="50"/>
-      <c r="O43" s="50"/>
-      <c r="P43" s="50"/>
-      <c r="Q43" s="50"/>
+      <c r="A43" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="24"/>
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G43" s="24"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="K43" s="24"/>
+      <c r="L43" s="24"/>
+      <c r="M43" s="24"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
+      <c r="Q43" s="33"/>
+      <c r="R43" s="34"/>
     </row>
     <row r="44" spans="1:18">
-      <c r="B44" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="C44" s="60"/>
-      <c r="D44" s="60"/>
-      <c r="E44" s="61"/>
-      <c r="F44" s="51" t="s">
+      <c r="A44" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
+      <c r="D44" s="24"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="G44" s="51"/>
-      <c r="H44" s="51" t="s">
-        <v>56</v>
-      </c>
-      <c r="I44" s="52"/>
-      <c r="J44" s="53" t="s">
-        <v>51</v>
-      </c>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51">
+      <c r="I44" s="61"/>
+      <c r="J44" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K44" s="24"/>
+      <c r="L44" s="24">
         <v>2.5</v>
       </c>
-      <c r="M44" s="52"/>
-      <c r="N44" s="50"/>
-      <c r="O44" s="50"/>
-      <c r="P44" s="50"/>
-      <c r="Q44" s="50"/>
+      <c r="M44" s="24"/>
+      <c r="N44" s="32"/>
+      <c r="O44" s="33"/>
+      <c r="P44" s="33"/>
+      <c r="Q44" s="33"/>
+      <c r="R44" s="34"/>
     </row>
-    <row r="46" spans="1:18" ht="14.4">
-      <c r="A46" s="45" t="s">
+    <row r="46" spans="1:18">
+      <c r="A46" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="57"/>
+      <c r="C46" s="57"/>
+      <c r="D46" s="57"/>
+      <c r="E46" s="57"/>
+      <c r="F46" s="58"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="B46" s="46"/>
-      <c r="C46" s="46"/>
-      <c r="D46" s="46"/>
-      <c r="E46" s="46"/>
-      <c r="F46" s="47"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="48" t="s">
+      <c r="I46" s="59"/>
+      <c r="J46" s="59"/>
+      <c r="K46" s="59"/>
+      <c r="L46" s="60"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
-      <c r="K46" s="48"/>
-      <c r="L46" s="49"/>
-      <c r="M46" s="17"/>
-      <c r="N46" s="48" t="s">
-        <v>65</v>
-      </c>
-      <c r="O46" s="48"/>
-      <c r="P46" s="48"/>
-      <c r="Q46" s="48"/>
-      <c r="R46" s="49"/>
+      <c r="O46" s="59"/>
+      <c r="P46" s="59"/>
+      <c r="Q46" s="59"/>
+      <c r="R46" s="60"/>
     </row>
     <row r="47" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="42"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="43"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="43"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="43"/>
-      <c r="J47" s="43"/>
-      <c r="K47" s="43"/>
-      <c r="L47" s="43"/>
-      <c r="M47" s="43"/>
-      <c r="N47" s="43"/>
-      <c r="O47" s="43"/>
-      <c r="P47" s="43"/>
-      <c r="Q47" s="43"/>
-      <c r="R47" s="44"/>
+      <c r="B47" s="53"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="54"/>
+      <c r="K47" s="54"/>
+      <c r="L47" s="54"/>
+      <c r="M47" s="54"/>
+      <c r="N47" s="54"/>
+      <c r="O47" s="54"/>
+      <c r="P47" s="54"/>
+      <c r="Q47" s="54"/>
+      <c r="R47" s="55"/>
     </row>
     <row r="48" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A48" s="26"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
-      <c r="M48" s="27"/>
-      <c r="N48" s="27"/>
-      <c r="O48" s="27"/>
-      <c r="P48" s="27"/>
-      <c r="Q48" s="27"/>
-      <c r="R48" s="28"/>
+      <c r="A48" s="39"/>
+      <c r="B48" s="40"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="40"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="40"/>
+      <c r="I48" s="40"/>
+      <c r="J48" s="40"/>
+      <c r="K48" s="40"/>
+      <c r="L48" s="40"/>
+      <c r="M48" s="40"/>
+      <c r="N48" s="40"/>
+      <c r="O48" s="40"/>
+      <c r="P48" s="40"/>
+      <c r="Q48" s="40"/>
+      <c r="R48" s="41"/>
     </row>
     <row r="49" spans="1:18">
-      <c r="A49" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="B49" s="55"/>
-      <c r="C49" s="55"/>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
-      <c r="F49" s="55"/>
-      <c r="G49" s="55"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="56"/>
-      <c r="J49" s="54" t="s">
-        <v>68</v>
-      </c>
-      <c r="K49" s="55"/>
-      <c r="L49" s="55"/>
-      <c r="M49" s="55"/>
-      <c r="N49" s="55"/>
-      <c r="O49" s="55"/>
-      <c r="P49" s="55"/>
-      <c r="Q49" s="55"/>
-      <c r="R49" s="56"/>
+      <c r="A49" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="63"/>
+      <c r="C49" s="63"/>
+      <c r="D49" s="63"/>
+      <c r="E49" s="63"/>
+      <c r="F49" s="63"/>
+      <c r="G49" s="63"/>
+      <c r="H49" s="63"/>
+      <c r="I49" s="64"/>
+      <c r="J49" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="K49" s="63"/>
+      <c r="L49" s="63"/>
+      <c r="M49" s="63"/>
+      <c r="N49" s="63"/>
+      <c r="O49" s="63"/>
+      <c r="P49" s="63"/>
+      <c r="Q49" s="63"/>
+      <c r="R49" s="64"/>
     </row>
     <row r="50" spans="1:18">
-      <c r="A50" s="57" t="s">
-        <v>67</v>
-      </c>
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="59"/>
-      <c r="J50" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="K50" s="58"/>
-      <c r="L50" s="58"/>
-      <c r="M50" s="58"/>
-      <c r="N50" s="58"/>
-      <c r="O50" s="58"/>
-      <c r="P50" s="58"/>
-      <c r="Q50" s="58"/>
-      <c r="R50" s="59"/>
+      <c r="A50" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B50" s="66"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="66"/>
+      <c r="E50" s="66"/>
+      <c r="F50" s="66"/>
+      <c r="G50" s="66"/>
+      <c r="H50" s="66"/>
+      <c r="I50" s="67"/>
+      <c r="J50" s="65" t="s">
+        <v>68</v>
+      </c>
+      <c r="K50" s="66"/>
+      <c r="L50" s="66"/>
+      <c r="M50" s="66"/>
+      <c r="N50" s="66"/>
+      <c r="O50" s="66"/>
+      <c r="P50" s="66"/>
+      <c r="Q50" s="66"/>
+      <c r="R50" s="67"/>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="23"/>
-      <c r="B51" s="24"/>
-      <c r="C51" s="24"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24"/>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="23"/>
-      <c r="K51" s="24"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
-      <c r="N51" s="24"/>
-      <c r="O51" s="24"/>
-      <c r="P51" s="24"/>
-      <c r="Q51" s="24"/>
-      <c r="R51" s="25"/>
+      <c r="A51" s="36"/>
+      <c r="B51" s="37"/>
+      <c r="C51" s="37"/>
+      <c r="D51" s="37"/>
+      <c r="E51" s="37"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="37"/>
+      <c r="H51" s="37"/>
+      <c r="I51" s="38"/>
+      <c r="J51" s="36"/>
+      <c r="K51" s="37"/>
+      <c r="L51" s="37"/>
+      <c r="M51" s="37"/>
+      <c r="N51" s="37"/>
+      <c r="O51" s="37"/>
+      <c r="P51" s="37"/>
+      <c r="Q51" s="37"/>
+      <c r="R51" s="38"/>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="23"/>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24"/>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="23"/>
-      <c r="K52" s="24"/>
-      <c r="L52" s="24"/>
-      <c r="M52" s="24"/>
-      <c r="N52" s="24"/>
-      <c r="O52" s="24"/>
-      <c r="P52" s="24"/>
-      <c r="Q52" s="24"/>
-      <c r="R52" s="25"/>
+      <c r="A52" s="36"/>
+      <c r="B52" s="37"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="37"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="37"/>
+      <c r="G52" s="37"/>
+      <c r="H52" s="37"/>
+      <c r="I52" s="38"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="37"/>
+      <c r="L52" s="37"/>
+      <c r="M52" s="37"/>
+      <c r="N52" s="37"/>
+      <c r="O52" s="37"/>
+      <c r="P52" s="37"/>
+      <c r="Q52" s="37"/>
+      <c r="R52" s="38"/>
     </row>
     <row r="53" spans="1:18">
-      <c r="A53" s="23"/>
-      <c r="B53" s="24"/>
-      <c r="C53" s="24"/>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24"/>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="23"/>
-      <c r="K53" s="24"/>
-      <c r="L53" s="24"/>
-      <c r="M53" s="24"/>
-      <c r="N53" s="24"/>
-      <c r="O53" s="24"/>
-      <c r="P53" s="24"/>
-      <c r="Q53" s="24"/>
-      <c r="R53" s="25"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="37"/>
+      <c r="C53" s="37"/>
+      <c r="D53" s="37"/>
+      <c r="E53" s="37"/>
+      <c r="F53" s="37"/>
+      <c r="G53" s="37"/>
+      <c r="H53" s="37"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="36"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="37"/>
+      <c r="M53" s="37"/>
+      <c r="N53" s="37"/>
+      <c r="O53" s="37"/>
+      <c r="P53" s="37"/>
+      <c r="Q53" s="37"/>
+      <c r="R53" s="38"/>
     </row>
     <row r="54" spans="1:18">
-      <c r="A54" s="23"/>
-      <c r="B54" s="24"/>
-      <c r="C54" s="24"/>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24"/>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="23"/>
-      <c r="K54" s="24"/>
-      <c r="L54" s="24"/>
-      <c r="M54" s="24"/>
-      <c r="N54" s="24"/>
-      <c r="O54" s="24"/>
-      <c r="P54" s="24"/>
-      <c r="Q54" s="24"/>
-      <c r="R54" s="25"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="37"/>
+      <c r="C54" s="37"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="36"/>
+      <c r="K54" s="37"/>
+      <c r="L54" s="37"/>
+      <c r="M54" s="37"/>
+      <c r="N54" s="37"/>
+      <c r="O54" s="37"/>
+      <c r="P54" s="37"/>
+      <c r="Q54" s="37"/>
+      <c r="R54" s="38"/>
     </row>
     <row r="55" spans="1:18">
-      <c r="A55" s="23"/>
-      <c r="B55" s="24"/>
-      <c r="C55" s="24"/>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24"/>
-      <c r="I55" s="25"/>
-      <c r="J55" s="23"/>
-      <c r="K55" s="24"/>
-      <c r="L55" s="24"/>
-      <c r="M55" s="24"/>
-      <c r="N55" s="24"/>
-      <c r="O55" s="24"/>
-      <c r="P55" s="24"/>
-      <c r="Q55" s="24"/>
-      <c r="R55" s="25"/>
+      <c r="A55" s="36"/>
+      <c r="B55" s="37"/>
+      <c r="C55" s="37"/>
+      <c r="D55" s="37"/>
+      <c r="E55" s="37"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="37"/>
+      <c r="H55" s="37"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="36"/>
+      <c r="K55" s="37"/>
+      <c r="L55" s="37"/>
+      <c r="M55" s="37"/>
+      <c r="N55" s="37"/>
+      <c r="O55" s="37"/>
+      <c r="P55" s="37"/>
+      <c r="Q55" s="37"/>
+      <c r="R55" s="38"/>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" s="26"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="27"/>
-      <c r="D56" s="27"/>
-      <c r="E56" s="27"/>
-      <c r="F56" s="27"/>
-      <c r="G56" s="27"/>
-      <c r="H56" s="27"/>
-      <c r="I56" s="28"/>
-      <c r="J56" s="26"/>
-      <c r="K56" s="27"/>
-      <c r="L56" s="27"/>
-      <c r="M56" s="27"/>
-      <c r="N56" s="27"/>
-      <c r="O56" s="27"/>
-      <c r="P56" s="27"/>
-      <c r="Q56" s="27"/>
-      <c r="R56" s="28"/>
+      <c r="A56" s="39"/>
+      <c r="B56" s="40"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="40"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="40"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="39"/>
+      <c r="K56" s="40"/>
+      <c r="L56" s="40"/>
+      <c r="M56" s="40"/>
+      <c r="N56" s="40"/>
+      <c r="O56" s="40"/>
+      <c r="P56" s="40"/>
+      <c r="Q56" s="40"/>
+      <c r="R56" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="107">
+  <mergeCells count="106">
     <mergeCell ref="I6:J7"/>
     <mergeCell ref="K6:L7"/>
     <mergeCell ref="M6:N7"/>
@@ -5600,10 +5756,6 @@
     <mergeCell ref="N27:N28"/>
     <mergeCell ref="O27:O28"/>
     <mergeCell ref="A30:C32"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="F37:M37"/>
     <mergeCell ref="N33:R33"/>
     <mergeCell ref="A34:C35"/>
     <mergeCell ref="D34:F35"/>
@@ -5615,28 +5767,10 @@
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="D33:H33"/>
     <mergeCell ref="I33:M33"/>
-    <mergeCell ref="B37:E37"/>
-    <mergeCell ref="B38:E38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:E40"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B43:E43"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
     <mergeCell ref="A49:I49"/>
     <mergeCell ref="A50:I50"/>
     <mergeCell ref="J49:R49"/>
     <mergeCell ref="J50:R50"/>
-    <mergeCell ref="B44:E44"/>
-    <mergeCell ref="N37:Q37"/>
-    <mergeCell ref="N38:Q38"/>
-    <mergeCell ref="N39:Q39"/>
-    <mergeCell ref="N40:Q40"/>
-    <mergeCell ref="N41:Q41"/>
-    <mergeCell ref="N42:Q42"/>
-    <mergeCell ref="N43:Q43"/>
     <mergeCell ref="J40:M40"/>
     <mergeCell ref="J41:M41"/>
     <mergeCell ref="J42:M42"/>
@@ -5646,6 +5780,10 @@
     <mergeCell ref="F40:I40"/>
     <mergeCell ref="F41:I41"/>
     <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="A38:E38"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="A51:I56"/>
     <mergeCell ref="J51:R56"/>
@@ -5668,11 +5806,28 @@
     <mergeCell ref="A46:F46"/>
     <mergeCell ref="H46:L46"/>
     <mergeCell ref="N46:R46"/>
-    <mergeCell ref="N44:Q44"/>
     <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="A39:E39"/>
+    <mergeCell ref="A40:E40"/>
+    <mergeCell ref="A41:E41"/>
+    <mergeCell ref="A42:E42"/>
+    <mergeCell ref="A43:E43"/>
+    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="N37:R37"/>
+    <mergeCell ref="N38:R38"/>
+    <mergeCell ref="N39:R39"/>
+    <mergeCell ref="N40:R40"/>
+    <mergeCell ref="N41:R41"/>
+    <mergeCell ref="N42:R42"/>
+    <mergeCell ref="N43:R43"/>
+    <mergeCell ref="N44:R44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
+    <mergeCell ref="A37:E37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="97" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C
 &amp;R&amp;G</oddHeader>
@@ -5693,14 +5848,246 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="B2" sqref="B2:Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="2" spans="2:17" ht="15" thickBot="1">
+      <c r="B2" s="132" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="132"/>
+      <c r="D2" s="132"/>
+      <c r="E2" s="133"/>
+      <c r="F2" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="132"/>
+      <c r="H2" s="132"/>
+      <c r="I2" s="132"/>
+      <c r="J2" s="132"/>
+      <c r="K2" s="132"/>
+      <c r="L2" s="132"/>
+      <c r="M2" s="132"/>
+      <c r="N2" s="132" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" s="132"/>
+      <c r="P2" s="132"/>
+      <c r="Q2" s="132"/>
+    </row>
+    <row r="3" spans="2:17">
+      <c r="B3" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="69"/>
+      <c r="D3" s="69"/>
+      <c r="E3" s="134"/>
+      <c r="F3" s="135" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="135"/>
+      <c r="H3" s="135"/>
+      <c r="I3" s="135"/>
+      <c r="J3" s="135" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="135"/>
+      <c r="L3" s="135"/>
+      <c r="M3" s="136"/>
+      <c r="N3" s="137"/>
+      <c r="O3" s="137"/>
+      <c r="P3" s="137"/>
+      <c r="Q3" s="137"/>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="B4" s="130" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="130"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="131"/>
+      <c r="F4" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="94"/>
+      <c r="O4" s="94"/>
+      <c r="P4" s="94"/>
+      <c r="Q4" s="94"/>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="130" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="130"/>
+      <c r="D5" s="130"/>
+      <c r="E5" s="131"/>
+      <c r="F5" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="24"/>
+      <c r="J5" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="24"/>
+      <c r="L5" s="24"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="94"/>
+      <c r="O5" s="94"/>
+      <c r="P5" s="94"/>
+      <c r="Q5" s="94"/>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="B6" s="130" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="130"/>
+      <c r="D6" s="130"/>
+      <c r="E6" s="131"/>
+      <c r="F6" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="61"/>
+      <c r="J6" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="24"/>
+      <c r="L6" s="24"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="94"/>
+      <c r="O6" s="94"/>
+      <c r="P6" s="94"/>
+      <c r="Q6" s="94"/>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="130" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="130"/>
+      <c r="D7" s="130"/>
+      <c r="E7" s="131"/>
+      <c r="F7" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="94"/>
+      <c r="O7" s="94"/>
+      <c r="P7" s="94"/>
+      <c r="Q7" s="94"/>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" s="130" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="130"/>
+      <c r="D8" s="130"/>
+      <c r="E8" s="131"/>
+      <c r="F8" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="24"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="94"/>
+      <c r="O8" s="94"/>
+      <c r="P8" s="94"/>
+      <c r="Q8" s="94"/>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="B9" s="130" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="130"/>
+      <c r="D9" s="130"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="61"/>
+      <c r="J9" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24">
+        <v>2.5</v>
+      </c>
+      <c r="M9" s="61"/>
+      <c r="N9" s="94"/>
+      <c r="O9" s="94"/>
+      <c r="P9" s="94"/>
+      <c r="Q9" s="94"/>
+    </row>
+  </sheetData>
+  <mergeCells count="33">
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="B8:E8"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="B9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="N9:Q9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Utworzenie algorytmu wyszukującego materiału pasujący do pozycji z boma. Poprawa wzorów kart kontroli łożysk garnkowych.
</commit_message>
<xml_diff>
--- a/data/wzor_PF.xlsx
+++ b/data/wzor_PF.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
   <si>
     <t>WYMIAR KONTROLNY</t>
   </si>
@@ -502,11 +502,14 @@
   <si>
     <t>-</t>
   </si>
+  <si>
+    <t>TWARDOŚĆ: Sh⁰A 50 +/-5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;zł&quot;_-;\-* #,##0.00\ &quot;zł&quot;_-;_-* &quot;-&quot;??\ &quot;zł&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
@@ -846,7 +849,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1448,6 +1451,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2554,7 +2619,7 @@
     <xf numFmtId="44" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="145">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2614,11 +2679,302 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2650,335 +3006,74 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1101">
@@ -4117,7 +4212,7 @@
         <xdr:cNvPr id="2" name="Skos 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4187,7 +4282,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>169815</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>138480</xdr:rowOff>
+      <xdr:rowOff>138481</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4225,7 +4320,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>109074</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>38832</xdr:rowOff>
+      <xdr:rowOff>38833</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4263,7 +4358,7 @@
       <xdr:col>16</xdr:col>
       <xdr:colOff>272424</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>146002</xdr:rowOff>
+      <xdr:rowOff>146003</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4274,7 +4369,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns="" xmlns:wpc="http://schemas.microsoft.com/office/word/2010/wordprocessingCanvas" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:wp14="http://schemas.microsoft.com/office/word/2010/wordprocessingDrawing" xmlns:w10="urn:schemas-microsoft-com:office:word" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main" xmlns:w14="http://schemas.microsoft.com/office/word/2010/wordml" xmlns:wpg="http://schemas.microsoft.com/office/word/2010/wordprocessingGroup" xmlns:wpi="http://schemas.microsoft.com/office/word/2010/wordprocessingInk" xmlns:wps="http://schemas.microsoft.com/office/word/2010/wordprocessingShape" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:wne="http://schemas.microsoft.com/office/word/2006/wordml" xmlns:wp="http://schemas.openxmlformats.org/drawingml/2006/wordprocessingDrawing" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:ve="http://schemas.openxmlformats.org/markup-compatibility/2006" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -4317,7 +4412,7 @@
         <xdr:cNvPr id="10" name="Skos 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4376,6 +4471,47 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>114300</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>76200</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>409575</xdr:colOff>
+          <xdr:row>25</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1025"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -4454,6 +4590,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -4488,6 +4625,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -4663,14 +4801,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="J16" zoomScale="130" zoomScaleNormal="70" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25:G26"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScale="130" zoomScaleNormal="70" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30:M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="14.25"/>
@@ -4681,26 +4819,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35"/>
-      <c r="R2" s="35"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
+      <c r="J2" s="98"/>
+      <c r="K2" s="98"/>
+      <c r="L2" s="98"/>
+      <c r="M2" s="98"/>
+      <c r="N2" s="98"/>
+      <c r="O2" s="98"/>
+      <c r="P2" s="98"/>
+      <c r="Q2" s="98"/>
+      <c r="R2" s="98"/>
     </row>
     <row r="3" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
       <c r="A3" s="21"/>
@@ -4723,102 +4861,102 @@
       <c r="R3" s="21"/>
     </row>
     <row r="4" spans="1:18" ht="13.15" customHeight="1" thickTop="1">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="105" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43" t="s">
+      <c r="B4" s="106"/>
+      <c r="C4" s="106" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43" t="s">
+      <c r="D4" s="106"/>
+      <c r="E4" s="106" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43" t="s">
+      <c r="F4" s="106"/>
+      <c r="G4" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43" t="s">
+      <c r="H4" s="106"/>
+      <c r="I4" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43" t="s">
+      <c r="J4" s="106"/>
+      <c r="K4" s="106" t="s">
         <v>74</v>
       </c>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43" t="s">
+      <c r="L4" s="106"/>
+      <c r="M4" s="106" t="s">
         <v>75</v>
       </c>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43" t="s">
+      <c r="N4" s="106"/>
+      <c r="O4" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43" t="s">
+      <c r="P4" s="106"/>
+      <c r="Q4" s="106" t="s">
         <v>77</v>
       </c>
-      <c r="R4" s="46"/>
+      <c r="R4" s="109"/>
     </row>
-    <row r="5" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="47"/>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1">
+      <c r="A5" s="107"/>
+      <c r="B5" s="108"/>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="108"/>
+      <c r="F5" s="108"/>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="108"/>
+      <c r="K5" s="108"/>
+      <c r="L5" s="108"/>
+      <c r="M5" s="108"/>
+      <c r="N5" s="108"/>
+      <c r="O5" s="108"/>
+      <c r="P5" s="108"/>
+      <c r="Q5" s="108"/>
+      <c r="R5" s="110"/>
     </row>
     <row r="6" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A6" s="48"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="49"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="49"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="49"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
-      <c r="P6" s="49"/>
-      <c r="Q6" s="49"/>
-      <c r="R6" s="108"/>
+      <c r="A6" s="111"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="25"/>
     </row>
     <row r="7" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
-      <c r="A7" s="50"/>
-      <c r="B7" s="51"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="51"/>
-      <c r="K7" s="51"/>
-      <c r="L7" s="51"/>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
-      <c r="P7" s="51"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="109"/>
+      <c r="A7" s="112"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="24"/>
+      <c r="M7" s="24"/>
+      <c r="N7" s="24"/>
+      <c r="O7" s="24"/>
+      <c r="P7" s="24"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="26"/>
     </row>
     <row r="8" spans="1:18" ht="13.15" customHeight="1" thickTop="1">
       <c r="A8" s="18"/>
@@ -4872,9 +5010,9 @@
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
-      <c r="G20" s="129"/>
-      <c r="H20" s="129"/>
-      <c r="I20" s="129"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20"/>
@@ -4894,7 +5032,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="129"/>
+      <c r="I21" s="52"/>
       <c r="J21"/>
       <c r="K21"/>
       <c r="L21"/>
@@ -4917,12 +5055,12 @@
       <c r="I22" s="9"/>
     </row>
     <row r="23" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
-      <c r="A23" s="98" t="s">
+      <c r="A23" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="98"/>
-      <c r="C23" s="98"/>
-      <c r="D23" s="107"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="28"/>
       <c r="E23" s="15" t="s">
         <v>8</v>
       </c>
@@ -4967,12 +5105,12 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A24" s="110" t="s">
+      <c r="A24" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="110"/>
-      <c r="C24" s="110"/>
-      <c r="D24" s="111"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="16"/>
       <c r="F24" s="12"/>
       <c r="G24" s="12" t="s">
@@ -5005,278 +5143,278 @@
       <c r="R24" s="12"/>
     </row>
     <row r="25" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A25" s="112" t="s">
+      <c r="A25" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="113"/>
-      <c r="C25" s="113"/>
-      <c r="D25" s="114"/>
-      <c r="E25" s="138" t="s">
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="F25" s="138"/>
-      <c r="G25" s="139"/>
+      <c r="F25" s="37"/>
+      <c r="G25" s="38"/>
       <c r="H25" s="6">
         <v>0.5</v>
       </c>
-      <c r="I25" s="118" t="s">
+      <c r="I25" s="41" t="s">
         <v>22</v>
       </c>
       <c r="J25" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="K25" s="119" t="s">
+      <c r="K25" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="L25" s="121" t="s">
+      <c r="L25" s="44" t="s">
         <v>28</v>
       </c>
-      <c r="M25" s="122"/>
-      <c r="N25" s="123"/>
-      <c r="O25" s="127" t="s">
+      <c r="M25" s="45"/>
+      <c r="N25" s="46"/>
+      <c r="O25" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="P25" s="102" t="s">
+      <c r="P25" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="Q25" s="102" t="s">
+      <c r="Q25" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="R25" s="103" t="s">
+      <c r="R25" s="59" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A26" s="115"/>
-      <c r="B26" s="116"/>
-      <c r="C26" s="116"/>
-      <c r="D26" s="117"/>
-      <c r="E26" s="140"/>
-      <c r="F26" s="140"/>
-      <c r="G26" s="141"/>
+      <c r="A26" s="34"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
+      <c r="G26" s="40"/>
       <c r="H26" s="3">
         <v>-1</v>
       </c>
-      <c r="I26" s="118"/>
+      <c r="I26" s="41"/>
       <c r="J26" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K26" s="120"/>
-      <c r="L26" s="124"/>
-      <c r="M26" s="125"/>
-      <c r="N26" s="126"/>
-      <c r="O26" s="128"/>
-      <c r="P26" s="102"/>
-      <c r="Q26" s="102"/>
-      <c r="R26" s="103"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="48"/>
+      <c r="N26" s="49"/>
+      <c r="O26" s="51"/>
+      <c r="P26" s="58"/>
+      <c r="Q26" s="58"/>
+      <c r="R26" s="59"/>
     </row>
     <row r="27" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A27" s="96" t="s">
+      <c r="A27" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="96"/>
-      <c r="C27" s="96"/>
-      <c r="D27" s="104"/>
-      <c r="E27" s="105"/>
-      <c r="F27" s="106"/>
-      <c r="G27" s="106"/>
-      <c r="H27" s="106"/>
-      <c r="I27" s="106"/>
-      <c r="J27" s="144"/>
-      <c r="K27" s="144"/>
-      <c r="L27" s="142" t="s">
+      <c r="B27" s="54"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="53"/>
+      <c r="K27" s="53"/>
+      <c r="L27" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="M27" s="142" t="s">
+      <c r="M27" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="N27" s="142" t="s">
+      <c r="N27" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="O27" s="144" t="s">
+      <c r="O27" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="P27" s="144" t="s">
+      <c r="P27" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="Q27" s="144" t="s">
+      <c r="Q27" s="53" t="s">
         <v>80</v>
       </c>
-      <c r="R27" s="144"/>
+      <c r="R27" s="53"/>
     </row>
     <row r="28" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A28" s="96"/>
-      <c r="B28" s="96"/>
-      <c r="C28" s="96"/>
-      <c r="D28" s="104"/>
-      <c r="E28" s="105"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="106"/>
-      <c r="H28" s="106"/>
-      <c r="I28" s="106"/>
-      <c r="J28" s="144"/>
-      <c r="K28" s="144"/>
-      <c r="L28" s="143"/>
-      <c r="M28" s="143"/>
-      <c r="N28" s="143"/>
-      <c r="O28" s="144"/>
-      <c r="P28" s="144"/>
-      <c r="Q28" s="144"/>
-      <c r="R28" s="144"/>
+      <c r="A28" s="54"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="60"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="64"/>
+      <c r="M28" s="64"/>
+      <c r="N28" s="64"/>
+      <c r="O28" s="53"/>
+      <c r="P28" s="53"/>
+      <c r="Q28" s="53"/>
+      <c r="R28" s="53"/>
     </row>
     <row r="29" spans="1:18" ht="13.15" customHeight="1"/>
     <row r="30" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A30" s="96" t="s">
+      <c r="A30" s="54" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="96"/>
-      <c r="C30" s="104"/>
-      <c r="D30" s="95" t="s">
+      <c r="B30" s="54"/>
+      <c r="C30" s="60"/>
+      <c r="D30" s="143" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="96"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="96"/>
-      <c r="H30" s="96"/>
-      <c r="I30" s="96" t="s">
+      <c r="E30" s="144"/>
+      <c r="F30" s="144"/>
+      <c r="G30" s="144"/>
+      <c r="H30" s="145"/>
+      <c r="I30" s="152" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="96"/>
-      <c r="K30" s="96"/>
-      <c r="L30" s="96"/>
-      <c r="M30" s="96"/>
-      <c r="N30" s="99" t="s">
+      <c r="J30" s="144"/>
+      <c r="K30" s="144"/>
+      <c r="L30" s="144"/>
+      <c r="M30" s="145"/>
+      <c r="N30" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="O30" s="100"/>
-      <c r="P30" s="100"/>
-      <c r="Q30" s="100"/>
-      <c r="R30" s="100"/>
+      <c r="O30" s="56"/>
+      <c r="P30" s="56"/>
+      <c r="Q30" s="56"/>
+      <c r="R30" s="56"/>
     </row>
     <row r="31" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A31" s="96"/>
-      <c r="B31" s="96"/>
-      <c r="C31" s="104"/>
-      <c r="D31" s="95"/>
-      <c r="E31" s="96"/>
-      <c r="F31" s="96"/>
-      <c r="G31" s="96"/>
-      <c r="H31" s="96"/>
-      <c r="I31" s="96"/>
-      <c r="J31" s="96"/>
-      <c r="K31" s="96"/>
-      <c r="L31" s="96"/>
-      <c r="M31" s="96"/>
-      <c r="N31" s="100"/>
-      <c r="O31" s="100"/>
-      <c r="P31" s="100"/>
-      <c r="Q31" s="100"/>
-      <c r="R31" s="100"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="146"/>
+      <c r="E31" s="147"/>
+      <c r="F31" s="147"/>
+      <c r="G31" s="147"/>
+      <c r="H31" s="148"/>
+      <c r="I31" s="153"/>
+      <c r="J31" s="147"/>
+      <c r="K31" s="147"/>
+      <c r="L31" s="147"/>
+      <c r="M31" s="148"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="P31" s="56"/>
+      <c r="Q31" s="56"/>
+      <c r="R31" s="56"/>
     </row>
     <row r="32" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
-      <c r="A32" s="98"/>
-      <c r="B32" s="98"/>
-      <c r="C32" s="107"/>
-      <c r="D32" s="97"/>
-      <c r="E32" s="98"/>
-      <c r="F32" s="98"/>
-      <c r="G32" s="98"/>
-      <c r="H32" s="98"/>
-      <c r="I32" s="98"/>
-      <c r="J32" s="98"/>
-      <c r="K32" s="98"/>
-      <c r="L32" s="98"/>
-      <c r="M32" s="98"/>
-      <c r="N32" s="101"/>
-      <c r="O32" s="101"/>
-      <c r="P32" s="101"/>
-      <c r="Q32" s="101"/>
-      <c r="R32" s="101"/>
+      <c r="A32" s="27"/>
+      <c r="B32" s="27"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="149"/>
+      <c r="E32" s="150"/>
+      <c r="F32" s="150"/>
+      <c r="G32" s="150"/>
+      <c r="H32" s="151"/>
+      <c r="I32" s="154"/>
+      <c r="J32" s="150"/>
+      <c r="K32" s="150"/>
+      <c r="L32" s="150"/>
+      <c r="M32" s="151"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="57"/>
+      <c r="P32" s="57"/>
+      <c r="Q32" s="57"/>
+      <c r="R32" s="57"/>
     </row>
     <row r="33" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
-      <c r="A33" s="85" t="s">
+      <c r="A33" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="85"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="87" t="s">
+      <c r="B33" s="81"/>
+      <c r="C33" s="82"/>
+      <c r="D33" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="88"/>
-      <c r="F33" s="88"/>
-      <c r="G33" s="89"/>
-      <c r="H33" s="89"/>
-      <c r="I33" s="88" t="s">
+      <c r="E33" s="84"/>
+      <c r="F33" s="84"/>
+      <c r="G33" s="85"/>
+      <c r="H33" s="85"/>
+      <c r="I33" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="J33" s="88"/>
-      <c r="K33" s="88"/>
-      <c r="L33" s="89"/>
-      <c r="M33" s="89"/>
-      <c r="N33" s="69" t="s">
+      <c r="J33" s="84"/>
+      <c r="K33" s="84"/>
+      <c r="L33" s="85"/>
+      <c r="M33" s="85"/>
+      <c r="N33" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="O33" s="69"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="70"/>
-      <c r="R33" s="70"/>
+      <c r="O33" s="65"/>
+      <c r="P33" s="65"/>
+      <c r="Q33" s="66"/>
+      <c r="R33" s="66"/>
     </row>
     <row r="34" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A34" s="71" t="s">
+      <c r="A34" s="67" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="72"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="72" t="s">
+      <c r="B34" s="68"/>
+      <c r="C34" s="69"/>
+      <c r="D34" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="72"/>
-      <c r="F34" s="72"/>
-      <c r="G34" s="77"/>
-      <c r="H34" s="78"/>
-      <c r="I34" s="72" t="s">
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="73"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="J34" s="72"/>
-      <c r="K34" s="72"/>
-      <c r="L34" s="81"/>
-      <c r="M34" s="82"/>
-      <c r="N34" s="72" t="s">
+      <c r="J34" s="68"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="77"/>
+      <c r="M34" s="78"/>
+      <c r="N34" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="O34" s="72"/>
-      <c r="P34" s="72"/>
-      <c r="Q34" s="81"/>
-      <c r="R34" s="82"/>
+      <c r="O34" s="68"/>
+      <c r="P34" s="68"/>
+      <c r="Q34" s="77"/>
+      <c r="R34" s="78"/>
     </row>
     <row r="35" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
-      <c r="A35" s="74"/>
-      <c r="B35" s="75"/>
-      <c r="C35" s="76"/>
-      <c r="D35" s="75"/>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="80"/>
-      <c r="I35" s="75"/>
-      <c r="J35" s="75"/>
-      <c r="K35" s="75"/>
-      <c r="L35" s="83"/>
-      <c r="M35" s="84"/>
-      <c r="N35" s="75"/>
-      <c r="O35" s="75"/>
-      <c r="P35" s="75"/>
-      <c r="Q35" s="83"/>
-      <c r="R35" s="84"/>
+      <c r="A35" s="70"/>
+      <c r="B35" s="71"/>
+      <c r="C35" s="72"/>
+      <c r="D35" s="71"/>
+      <c r="E35" s="71"/>
+      <c r="F35" s="71"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="76"/>
+      <c r="I35" s="71"/>
+      <c r="J35" s="71"/>
+      <c r="K35" s="71"/>
+      <c r="L35" s="79"/>
+      <c r="M35" s="80"/>
+      <c r="N35" s="71"/>
+      <c r="O35" s="71"/>
+      <c r="P35" s="71"/>
+      <c r="Q35" s="79"/>
+      <c r="R35" s="80"/>
     </row>
     <row r="37" spans="1:18" ht="15" thickBot="1">
-      <c r="A37" s="90" t="s">
+      <c r="A37" s="132" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="27"/>
-      <c r="C37" s="27"/>
-      <c r="D37" s="27"/>
-      <c r="E37" s="91"/>
+      <c r="B37" s="124"/>
+      <c r="C37" s="124"/>
+      <c r="D37" s="124"/>
+      <c r="E37" s="133"/>
       <c r="F37" s="22" t="s">
         <v>2</v>
       </c>
@@ -5287,503 +5425,449 @@
       <c r="K37" s="22"/>
       <c r="L37" s="22"/>
       <c r="M37" s="22"/>
-      <c r="N37" s="26" t="s">
+      <c r="N37" s="123" t="s">
         <v>3</v>
       </c>
-      <c r="O37" s="27"/>
-      <c r="P37" s="27"/>
-      <c r="Q37" s="27"/>
-      <c r="R37" s="28"/>
+      <c r="O37" s="124"/>
+      <c r="P37" s="124"/>
+      <c r="Q37" s="124"/>
+      <c r="R37" s="125"/>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="92" t="s">
+      <c r="A38" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="68"/>
-      <c r="C38" s="68"/>
-      <c r="D38" s="68"/>
-      <c r="E38" s="93"/>
-      <c r="F38" s="68" t="s">
+      <c r="B38" s="94"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="97"/>
+      <c r="F38" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68" t="s">
+      <c r="G38" s="94"/>
+      <c r="H38" s="94"/>
+      <c r="I38" s="94"/>
+      <c r="J38" s="94" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="29"/>
-      <c r="O38" s="30"/>
-      <c r="P38" s="30"/>
-      <c r="Q38" s="30"/>
-      <c r="R38" s="31"/>
+      <c r="K38" s="94"/>
+      <c r="L38" s="94"/>
+      <c r="M38" s="94"/>
+      <c r="N38" s="126"/>
+      <c r="O38" s="127"/>
+      <c r="P38" s="127"/>
+      <c r="Q38" s="127"/>
+      <c r="R38" s="128"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="23" t="s">
+      <c r="A39" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="24" t="s">
+      <c r="B39" s="92"/>
+      <c r="C39" s="92"/>
+      <c r="D39" s="92"/>
+      <c r="E39" s="122"/>
+      <c r="F39" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="G39" s="24"/>
-      <c r="H39" s="24"/>
-      <c r="I39" s="24"/>
-      <c r="J39" s="24" t="s">
+      <c r="G39" s="92"/>
+      <c r="H39" s="92"/>
+      <c r="I39" s="92"/>
+      <c r="J39" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="K39" s="24"/>
-      <c r="L39" s="24"/>
-      <c r="M39" s="24"/>
-      <c r="N39" s="32"/>
-      <c r="O39" s="33"/>
-      <c r="P39" s="33"/>
-      <c r="Q39" s="33"/>
-      <c r="R39" s="34"/>
+      <c r="K39" s="92"/>
+      <c r="L39" s="92"/>
+      <c r="M39" s="92"/>
+      <c r="N39" s="129"/>
+      <c r="O39" s="130"/>
+      <c r="P39" s="130"/>
+      <c r="Q39" s="130"/>
+      <c r="R39" s="131"/>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="93" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="24" t="s">
+      <c r="B40" s="92"/>
+      <c r="C40" s="92"/>
+      <c r="D40" s="92"/>
+      <c r="E40" s="122"/>
+      <c r="F40" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="G40" s="24"/>
-      <c r="H40" s="24"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24" t="s">
+      <c r="G40" s="92"/>
+      <c r="H40" s="92"/>
+      <c r="I40" s="92"/>
+      <c r="J40" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
-      <c r="R40" s="34"/>
+      <c r="K40" s="92"/>
+      <c r="L40" s="92"/>
+      <c r="M40" s="92"/>
+      <c r="N40" s="129"/>
+      <c r="O40" s="130"/>
+      <c r="P40" s="130"/>
+      <c r="Q40" s="130"/>
+      <c r="R40" s="131"/>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="93" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="24"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="24" t="s">
+      <c r="B41" s="92"/>
+      <c r="C41" s="92"/>
+      <c r="D41" s="92"/>
+      <c r="E41" s="122"/>
+      <c r="F41" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="G41" s="24"/>
-      <c r="H41" s="24"/>
-      <c r="I41" s="61"/>
-      <c r="J41" s="23" t="s">
+      <c r="G41" s="92"/>
+      <c r="H41" s="92"/>
+      <c r="I41" s="95"/>
+      <c r="J41" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="K41" s="24"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="24"/>
-      <c r="N41" s="32"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
-      <c r="R41" s="34"/>
+      <c r="K41" s="92"/>
+      <c r="L41" s="92"/>
+      <c r="M41" s="92"/>
+      <c r="N41" s="129"/>
+      <c r="O41" s="130"/>
+      <c r="P41" s="130"/>
+      <c r="Q41" s="130"/>
+      <c r="R41" s="131"/>
     </row>
     <row r="42" spans="1:18">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="24"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="24" t="s">
+      <c r="B42" s="92"/>
+      <c r="C42" s="92"/>
+      <c r="D42" s="92"/>
+      <c r="E42" s="122"/>
+      <c r="F42" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="G42" s="24"/>
-      <c r="H42" s="24"/>
-      <c r="I42" s="61"/>
-      <c r="J42" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="K42" s="24"/>
-      <c r="L42" s="24"/>
-      <c r="M42" s="24"/>
-      <c r="N42" s="32"/>
-      <c r="O42" s="33"/>
-      <c r="P42" s="33"/>
-      <c r="Q42" s="33"/>
-      <c r="R42" s="34"/>
+      <c r="G42" s="92"/>
+      <c r="H42" s="92"/>
+      <c r="I42" s="95"/>
+      <c r="J42" s="93" t="s">
+        <v>81</v>
+      </c>
+      <c r="K42" s="92"/>
+      <c r="L42" s="92"/>
+      <c r="M42" s="92"/>
+      <c r="N42" s="129"/>
+      <c r="O42" s="130"/>
+      <c r="P42" s="130"/>
+      <c r="Q42" s="130"/>
+      <c r="R42" s="131"/>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="24"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="24" t="s">
+      <c r="B43" s="92"/>
+      <c r="C43" s="92"/>
+      <c r="D43" s="92"/>
+      <c r="E43" s="122"/>
+      <c r="F43" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="G43" s="24"/>
-      <c r="H43" s="24"/>
-      <c r="I43" s="24"/>
-      <c r="J43" s="24" t="s">
+      <c r="G43" s="92"/>
+      <c r="H43" s="92"/>
+      <c r="I43" s="92"/>
+      <c r="J43" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="K43" s="24"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="24"/>
-      <c r="N43" s="32"/>
-      <c r="O43" s="33"/>
-      <c r="P43" s="33"/>
-      <c r="Q43" s="33"/>
-      <c r="R43" s="34"/>
+      <c r="K43" s="92"/>
+      <c r="L43" s="92"/>
+      <c r="M43" s="92"/>
+      <c r="N43" s="129"/>
+      <c r="O43" s="130"/>
+      <c r="P43" s="130"/>
+      <c r="Q43" s="130"/>
+      <c r="R43" s="131"/>
     </row>
     <row r="44" spans="1:18">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="93" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="24" t="s">
+      <c r="B44" s="92"/>
+      <c r="C44" s="92"/>
+      <c r="D44" s="92"/>
+      <c r="E44" s="122"/>
+      <c r="F44" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24" t="s">
+      <c r="G44" s="92"/>
+      <c r="H44" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="I44" s="61"/>
-      <c r="J44" s="23" t="s">
+      <c r="I44" s="95"/>
+      <c r="J44" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="K44" s="24"/>
-      <c r="L44" s="24">
+      <c r="K44" s="92"/>
+      <c r="L44" s="92">
         <v>2.5</v>
       </c>
-      <c r="M44" s="24"/>
-      <c r="N44" s="32"/>
-      <c r="O44" s="33"/>
-      <c r="P44" s="33"/>
-      <c r="Q44" s="33"/>
-      <c r="R44" s="34"/>
+      <c r="M44" s="92"/>
+      <c r="N44" s="129"/>
+      <c r="O44" s="130"/>
+      <c r="P44" s="130"/>
+      <c r="Q44" s="130"/>
+      <c r="R44" s="131"/>
     </row>
     <row r="46" spans="1:18">
-      <c r="A46" s="56" t="s">
+      <c r="A46" s="117" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
-      <c r="E46" s="57"/>
-      <c r="F46" s="58"/>
+      <c r="B46" s="118"/>
+      <c r="C46" s="118"/>
+      <c r="D46" s="118"/>
+      <c r="E46" s="118"/>
+      <c r="F46" s="119"/>
       <c r="G46" s="17"/>
-      <c r="H46" s="59" t="s">
+      <c r="H46" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="I46" s="59"/>
-      <c r="J46" s="59"/>
-      <c r="K46" s="59"/>
-      <c r="L46" s="60"/>
+      <c r="I46" s="120"/>
+      <c r="J46" s="120"/>
+      <c r="K46" s="120"/>
+      <c r="L46" s="121"/>
       <c r="M46" s="17"/>
-      <c r="N46" s="59" t="s">
+      <c r="N46" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="O46" s="59"/>
-      <c r="P46" s="59"/>
-      <c r="Q46" s="59"/>
-      <c r="R46" s="60"/>
+      <c r="O46" s="120"/>
+      <c r="P46" s="120"/>
+      <c r="Q46" s="120"/>
+      <c r="R46" s="121"/>
     </row>
     <row r="47" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A47" s="52" t="s">
+      <c r="A47" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="53"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="54"/>
-      <c r="E47" s="54"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="54"/>
-      <c r="H47" s="54"/>
-      <c r="I47" s="54"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="54"/>
-      <c r="L47" s="54"/>
-      <c r="M47" s="54"/>
-      <c r="N47" s="54"/>
-      <c r="O47" s="54"/>
-      <c r="P47" s="54"/>
-      <c r="Q47" s="54"/>
-      <c r="R47" s="55"/>
+      <c r="B47" s="114"/>
+      <c r="C47" s="115"/>
+      <c r="D47" s="115"/>
+      <c r="E47" s="115"/>
+      <c r="F47" s="115"/>
+      <c r="G47" s="115"/>
+      <c r="H47" s="115"/>
+      <c r="I47" s="115"/>
+      <c r="J47" s="115"/>
+      <c r="K47" s="115"/>
+      <c r="L47" s="115"/>
+      <c r="M47" s="115"/>
+      <c r="N47" s="115"/>
+      <c r="O47" s="115"/>
+      <c r="P47" s="115"/>
+      <c r="Q47" s="115"/>
+      <c r="R47" s="116"/>
     </row>
     <row r="48" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A48" s="39"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="40"/>
-      <c r="G48" s="40"/>
-      <c r="H48" s="40"/>
-      <c r="I48" s="40"/>
-      <c r="J48" s="40"/>
-      <c r="K48" s="40"/>
-      <c r="L48" s="40"/>
-      <c r="M48" s="40"/>
-      <c r="N48" s="40"/>
-      <c r="O48" s="40"/>
-      <c r="P48" s="40"/>
-      <c r="Q48" s="40"/>
-      <c r="R48" s="41"/>
+      <c r="A48" s="102"/>
+      <c r="B48" s="103"/>
+      <c r="C48" s="103"/>
+      <c r="D48" s="103"/>
+      <c r="E48" s="103"/>
+      <c r="F48" s="103"/>
+      <c r="G48" s="103"/>
+      <c r="H48" s="103"/>
+      <c r="I48" s="103"/>
+      <c r="J48" s="103"/>
+      <c r="K48" s="103"/>
+      <c r="L48" s="103"/>
+      <c r="M48" s="103"/>
+      <c r="N48" s="103"/>
+      <c r="O48" s="103"/>
+      <c r="P48" s="103"/>
+      <c r="Q48" s="103"/>
+      <c r="R48" s="104"/>
     </row>
     <row r="49" spans="1:18">
-      <c r="A49" s="62" t="s">
+      <c r="A49" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="B49" s="63"/>
-      <c r="C49" s="63"/>
-      <c r="D49" s="63"/>
-      <c r="E49" s="63"/>
-      <c r="F49" s="63"/>
-      <c r="G49" s="63"/>
-      <c r="H49" s="63"/>
-      <c r="I49" s="64"/>
-      <c r="J49" s="62" t="s">
+      <c r="B49" s="87"/>
+      <c r="C49" s="87"/>
+      <c r="D49" s="87"/>
+      <c r="E49" s="87"/>
+      <c r="F49" s="87"/>
+      <c r="G49" s="87"/>
+      <c r="H49" s="87"/>
+      <c r="I49" s="88"/>
+      <c r="J49" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="K49" s="63"/>
-      <c r="L49" s="63"/>
-      <c r="M49" s="63"/>
-      <c r="N49" s="63"/>
-      <c r="O49" s="63"/>
-      <c r="P49" s="63"/>
-      <c r="Q49" s="63"/>
-      <c r="R49" s="64"/>
+      <c r="K49" s="87"/>
+      <c r="L49" s="87"/>
+      <c r="M49" s="87"/>
+      <c r="N49" s="87"/>
+      <c r="O49" s="87"/>
+      <c r="P49" s="87"/>
+      <c r="Q49" s="87"/>
+      <c r="R49" s="88"/>
     </row>
     <row r="50" spans="1:18">
-      <c r="A50" s="65" t="s">
+      <c r="A50" s="89" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="66"/>
-      <c r="C50" s="66"/>
-      <c r="D50" s="66"/>
-      <c r="E50" s="66"/>
-      <c r="F50" s="66"/>
-      <c r="G50" s="66"/>
-      <c r="H50" s="66"/>
-      <c r="I50" s="67"/>
-      <c r="J50" s="65" t="s">
+      <c r="B50" s="90"/>
+      <c r="C50" s="90"/>
+      <c r="D50" s="90"/>
+      <c r="E50" s="90"/>
+      <c r="F50" s="90"/>
+      <c r="G50" s="90"/>
+      <c r="H50" s="90"/>
+      <c r="I50" s="91"/>
+      <c r="J50" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="K50" s="66"/>
-      <c r="L50" s="66"/>
-      <c r="M50" s="66"/>
-      <c r="N50" s="66"/>
-      <c r="O50" s="66"/>
-      <c r="P50" s="66"/>
-      <c r="Q50" s="66"/>
-      <c r="R50" s="67"/>
+      <c r="K50" s="90"/>
+      <c r="L50" s="90"/>
+      <c r="M50" s="90"/>
+      <c r="N50" s="90"/>
+      <c r="O50" s="90"/>
+      <c r="P50" s="90"/>
+      <c r="Q50" s="90"/>
+      <c r="R50" s="91"/>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="36"/>
-      <c r="B51" s="37"/>
-      <c r="C51" s="37"/>
-      <c r="D51" s="37"/>
-      <c r="E51" s="37"/>
-      <c r="F51" s="37"/>
-      <c r="G51" s="37"/>
-      <c r="H51" s="37"/>
-      <c r="I51" s="38"/>
-      <c r="J51" s="36"/>
-      <c r="K51" s="37"/>
-      <c r="L51" s="37"/>
-      <c r="M51" s="37"/>
-      <c r="N51" s="37"/>
-      <c r="O51" s="37"/>
-      <c r="P51" s="37"/>
-      <c r="Q51" s="37"/>
-      <c r="R51" s="38"/>
+      <c r="A51" s="99"/>
+      <c r="B51" s="100"/>
+      <c r="C51" s="100"/>
+      <c r="D51" s="100"/>
+      <c r="E51" s="100"/>
+      <c r="F51" s="100"/>
+      <c r="G51" s="100"/>
+      <c r="H51" s="100"/>
+      <c r="I51" s="101"/>
+      <c r="J51" s="99"/>
+      <c r="K51" s="100"/>
+      <c r="L51" s="100"/>
+      <c r="M51" s="100"/>
+      <c r="N51" s="100"/>
+      <c r="O51" s="100"/>
+      <c r="P51" s="100"/>
+      <c r="Q51" s="100"/>
+      <c r="R51" s="101"/>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="36"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="37"/>
-      <c r="D52" s="37"/>
-      <c r="E52" s="37"/>
-      <c r="F52" s="37"/>
-      <c r="G52" s="37"/>
-      <c r="H52" s="37"/>
-      <c r="I52" s="38"/>
-      <c r="J52" s="36"/>
-      <c r="K52" s="37"/>
-      <c r="L52" s="37"/>
-      <c r="M52" s="37"/>
-      <c r="N52" s="37"/>
-      <c r="O52" s="37"/>
-      <c r="P52" s="37"/>
-      <c r="Q52" s="37"/>
-      <c r="R52" s="38"/>
+      <c r="A52" s="99"/>
+      <c r="B52" s="100"/>
+      <c r="C52" s="100"/>
+      <c r="D52" s="100"/>
+      <c r="E52" s="100"/>
+      <c r="F52" s="100"/>
+      <c r="G52" s="100"/>
+      <c r="H52" s="100"/>
+      <c r="I52" s="101"/>
+      <c r="J52" s="99"/>
+      <c r="K52" s="100"/>
+      <c r="L52" s="100"/>
+      <c r="M52" s="100"/>
+      <c r="N52" s="100"/>
+      <c r="O52" s="100"/>
+      <c r="P52" s="100"/>
+      <c r="Q52" s="100"/>
+      <c r="R52" s="101"/>
     </row>
     <row r="53" spans="1:18">
-      <c r="A53" s="36"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="37"/>
-      <c r="D53" s="37"/>
-      <c r="E53" s="37"/>
-      <c r="F53" s="37"/>
-      <c r="G53" s="37"/>
-      <c r="H53" s="37"/>
-      <c r="I53" s="38"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="37"/>
-      <c r="L53" s="37"/>
-      <c r="M53" s="37"/>
-      <c r="N53" s="37"/>
-      <c r="O53" s="37"/>
-      <c r="P53" s="37"/>
-      <c r="Q53" s="37"/>
-      <c r="R53" s="38"/>
+      <c r="A53" s="99"/>
+      <c r="B53" s="100"/>
+      <c r="C53" s="100"/>
+      <c r="D53" s="100"/>
+      <c r="E53" s="100"/>
+      <c r="F53" s="100"/>
+      <c r="G53" s="100"/>
+      <c r="H53" s="100"/>
+      <c r="I53" s="101"/>
+      <c r="J53" s="99"/>
+      <c r="K53" s="100"/>
+      <c r="L53" s="100"/>
+      <c r="M53" s="100"/>
+      <c r="N53" s="100"/>
+      <c r="O53" s="100"/>
+      <c r="P53" s="100"/>
+      <c r="Q53" s="100"/>
+      <c r="R53" s="101"/>
     </row>
     <row r="54" spans="1:18">
-      <c r="A54" s="36"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="37"/>
-      <c r="D54" s="37"/>
-      <c r="E54" s="37"/>
-      <c r="F54" s="37"/>
-      <c r="G54" s="37"/>
-      <c r="H54" s="37"/>
-      <c r="I54" s="38"/>
-      <c r="J54" s="36"/>
-      <c r="K54" s="37"/>
-      <c r="L54" s="37"/>
-      <c r="M54" s="37"/>
-      <c r="N54" s="37"/>
-      <c r="O54" s="37"/>
-      <c r="P54" s="37"/>
-      <c r="Q54" s="37"/>
-      <c r="R54" s="38"/>
+      <c r="A54" s="99"/>
+      <c r="B54" s="100"/>
+      <c r="C54" s="100"/>
+      <c r="D54" s="100"/>
+      <c r="E54" s="100"/>
+      <c r="F54" s="100"/>
+      <c r="G54" s="100"/>
+      <c r="H54" s="100"/>
+      <c r="I54" s="101"/>
+      <c r="J54" s="99"/>
+      <c r="K54" s="100"/>
+      <c r="L54" s="100"/>
+      <c r="M54" s="100"/>
+      <c r="N54" s="100"/>
+      <c r="O54" s="100"/>
+      <c r="P54" s="100"/>
+      <c r="Q54" s="100"/>
+      <c r="R54" s="101"/>
     </row>
     <row r="55" spans="1:18">
-      <c r="A55" s="36"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="37"/>
-      <c r="D55" s="37"/>
-      <c r="E55" s="37"/>
-      <c r="F55" s="37"/>
-      <c r="G55" s="37"/>
-      <c r="H55" s="37"/>
-      <c r="I55" s="38"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="37"/>
-      <c r="L55" s="37"/>
-      <c r="M55" s="37"/>
-      <c r="N55" s="37"/>
-      <c r="O55" s="37"/>
-      <c r="P55" s="37"/>
-      <c r="Q55" s="37"/>
-      <c r="R55" s="38"/>
+      <c r="A55" s="99"/>
+      <c r="B55" s="100"/>
+      <c r="C55" s="100"/>
+      <c r="D55" s="100"/>
+      <c r="E55" s="100"/>
+      <c r="F55" s="100"/>
+      <c r="G55" s="100"/>
+      <c r="H55" s="100"/>
+      <c r="I55" s="101"/>
+      <c r="J55" s="99"/>
+      <c r="K55" s="100"/>
+      <c r="L55" s="100"/>
+      <c r="M55" s="100"/>
+      <c r="N55" s="100"/>
+      <c r="O55" s="100"/>
+      <c r="P55" s="100"/>
+      <c r="Q55" s="100"/>
+      <c r="R55" s="101"/>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" s="39"/>
-      <c r="B56" s="40"/>
-      <c r="C56" s="40"/>
-      <c r="D56" s="40"/>
-      <c r="E56" s="40"/>
-      <c r="F56" s="40"/>
-      <c r="G56" s="40"/>
-      <c r="H56" s="40"/>
-      <c r="I56" s="41"/>
-      <c r="J56" s="39"/>
-      <c r="K56" s="40"/>
-      <c r="L56" s="40"/>
-      <c r="M56" s="40"/>
-      <c r="N56" s="40"/>
-      <c r="O56" s="40"/>
-      <c r="P56" s="40"/>
-      <c r="Q56" s="40"/>
-      <c r="R56" s="41"/>
+      <c r="A56" s="102"/>
+      <c r="B56" s="103"/>
+      <c r="C56" s="103"/>
+      <c r="D56" s="103"/>
+      <c r="E56" s="103"/>
+      <c r="F56" s="103"/>
+      <c r="G56" s="103"/>
+      <c r="H56" s="103"/>
+      <c r="I56" s="104"/>
+      <c r="J56" s="102"/>
+      <c r="K56" s="103"/>
+      <c r="L56" s="103"/>
+      <c r="M56" s="103"/>
+      <c r="N56" s="103"/>
+      <c r="O56" s="103"/>
+      <c r="P56" s="103"/>
+      <c r="Q56" s="103"/>
+      <c r="R56" s="104"/>
     </row>
   </sheetData>
   <mergeCells count="106">
-    <mergeCell ref="I6:J7"/>
-    <mergeCell ref="K6:L7"/>
-    <mergeCell ref="M6:N7"/>
-    <mergeCell ref="O6:P7"/>
-    <mergeCell ref="Q6:R7"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A25:D26"/>
-    <mergeCell ref="E25:G26"/>
-    <mergeCell ref="I25:I26"/>
-    <mergeCell ref="K25:K26"/>
-    <mergeCell ref="L25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="P27:P28"/>
-    <mergeCell ref="Q27:Q28"/>
-    <mergeCell ref="R27:R28"/>
-    <mergeCell ref="D30:H32"/>
-    <mergeCell ref="I30:M32"/>
-    <mergeCell ref="N30:R32"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q25:Q26"/>
-    <mergeCell ref="R25:R26"/>
-    <mergeCell ref="A27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="G27:G28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="J27:J28"/>
-    <mergeCell ref="K27:K28"/>
-    <mergeCell ref="L27:L28"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="N27:N28"/>
-    <mergeCell ref="O27:O28"/>
-    <mergeCell ref="A30:C32"/>
-    <mergeCell ref="N33:R33"/>
-    <mergeCell ref="A34:C35"/>
-    <mergeCell ref="D34:F35"/>
-    <mergeCell ref="G34:H35"/>
-    <mergeCell ref="I34:K35"/>
-    <mergeCell ref="L34:M35"/>
-    <mergeCell ref="N34:P35"/>
-    <mergeCell ref="Q34:R35"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="D33:H33"/>
-    <mergeCell ref="I33:M33"/>
-    <mergeCell ref="A49:I49"/>
-    <mergeCell ref="A50:I50"/>
-    <mergeCell ref="J49:R49"/>
-    <mergeCell ref="J50:R50"/>
-    <mergeCell ref="J40:M40"/>
-    <mergeCell ref="J41:M41"/>
-    <mergeCell ref="J42:M42"/>
-    <mergeCell ref="J43:M43"/>
-    <mergeCell ref="F38:I38"/>
-    <mergeCell ref="F39:I39"/>
-    <mergeCell ref="F40:I40"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="F43:I43"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="N37:R37"/>
+    <mergeCell ref="N38:R38"/>
+    <mergeCell ref="N39:R39"/>
+    <mergeCell ref="N40:R40"/>
+    <mergeCell ref="N41:R41"/>
+    <mergeCell ref="N42:R42"/>
+    <mergeCell ref="N43:R43"/>
+    <mergeCell ref="N44:R44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="L44:M44"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="A51:I56"/>
     <mergeCell ref="J51:R56"/>
@@ -5808,23 +5892,77 @@
     <mergeCell ref="N46:R46"/>
     <mergeCell ref="F44:G44"/>
     <mergeCell ref="H44:I44"/>
+    <mergeCell ref="A49:I49"/>
+    <mergeCell ref="A50:I50"/>
+    <mergeCell ref="J49:R49"/>
+    <mergeCell ref="J50:R50"/>
+    <mergeCell ref="J40:M40"/>
+    <mergeCell ref="J41:M41"/>
+    <mergeCell ref="J42:M42"/>
+    <mergeCell ref="J43:M43"/>
+    <mergeCell ref="F38:I38"/>
+    <mergeCell ref="F39:I39"/>
+    <mergeCell ref="F40:I40"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="F43:I43"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="A38:E38"/>
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="A40:E40"/>
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="A42:E42"/>
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="A44:E44"/>
-    <mergeCell ref="N37:R37"/>
-    <mergeCell ref="N38:R38"/>
-    <mergeCell ref="N39:R39"/>
-    <mergeCell ref="N40:R40"/>
-    <mergeCell ref="N41:R41"/>
-    <mergeCell ref="N42:R42"/>
-    <mergeCell ref="N43:R43"/>
-    <mergeCell ref="N44:R44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="L44:M44"/>
-    <mergeCell ref="A37:E37"/>
+    <mergeCell ref="N33:R33"/>
+    <mergeCell ref="A34:C35"/>
+    <mergeCell ref="D34:F35"/>
+    <mergeCell ref="G34:H35"/>
+    <mergeCell ref="I34:K35"/>
+    <mergeCell ref="L34:M35"/>
+    <mergeCell ref="N34:P35"/>
+    <mergeCell ref="Q34:R35"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="D33:H33"/>
+    <mergeCell ref="I33:M33"/>
+    <mergeCell ref="P27:P28"/>
+    <mergeCell ref="Q27:Q28"/>
+    <mergeCell ref="R27:R28"/>
+    <mergeCell ref="D30:H32"/>
+    <mergeCell ref="I30:M32"/>
+    <mergeCell ref="N30:R32"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q25:Q26"/>
+    <mergeCell ref="R25:R26"/>
+    <mergeCell ref="A27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="G27:G28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="J27:J28"/>
+    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="L27:L28"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="N27:N28"/>
+    <mergeCell ref="O27:O28"/>
+    <mergeCell ref="A30:C32"/>
+    <mergeCell ref="I6:J7"/>
+    <mergeCell ref="K6:L7"/>
+    <mergeCell ref="M6:N7"/>
+    <mergeCell ref="O6:P7"/>
+    <mergeCell ref="Q6:R7"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A25:D26"/>
+    <mergeCell ref="E25:G26"/>
+    <mergeCell ref="I25:I26"/>
+    <mergeCell ref="K25:K26"/>
+    <mergeCell ref="L25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="G20:H20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5841,13 +5979,37 @@
   <legacyDrawing r:id="rId3"/>
   <legacyDrawingHF r:id="rId4"/>
   <oleObjects>
-    <oleObject progId="Equation.3" shapeId="1025" r:id="rId5"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <oleObject progId="Equation.3" shapeId="1025" r:id="rId5">
+          <objectPr defaultSize="0" autoPict="0" r:id="rId6">
+            <anchor moveWithCells="1" sizeWithCells="1">
+              <from>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>114300</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>13</xdr:col>
+                <xdr:colOff>342900</xdr:colOff>
+                <xdr:row>26</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </objectPr>
+        </oleObject>
+      </mc:Choice>
+      <mc:Fallback>
+        <oleObject progId="Equation.3" shapeId="1025" r:id="rId5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
   </oleObjects>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5857,226 +6019,203 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="2" spans="2:17" ht="15" thickBot="1">
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
-      <c r="E2" s="133"/>
-      <c r="F2" s="28" t="s">
+      <c r="C2" s="134"/>
+      <c r="D2" s="134"/>
+      <c r="E2" s="135"/>
+      <c r="F2" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="132"/>
-      <c r="H2" s="132"/>
-      <c r="I2" s="132"/>
-      <c r="J2" s="132"/>
-      <c r="K2" s="132"/>
-      <c r="L2" s="132"/>
-      <c r="M2" s="132"/>
-      <c r="N2" s="132" t="s">
+      <c r="G2" s="134"/>
+      <c r="H2" s="134"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="134"/>
+      <c r="K2" s="134"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="134"/>
+      <c r="N2" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="132"/>
-      <c r="P2" s="132"/>
-      <c r="Q2" s="132"/>
+      <c r="O2" s="134"/>
+      <c r="P2" s="134"/>
+      <c r="Q2" s="134"/>
     </row>
     <row r="3" spans="2:17">
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="134"/>
-      <c r="F3" s="135" t="s">
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="136"/>
+      <c r="F3" s="137" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="135"/>
-      <c r="H3" s="135"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135" t="s">
+      <c r="G3" s="137"/>
+      <c r="H3" s="137"/>
+      <c r="I3" s="137"/>
+      <c r="J3" s="137" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="136"/>
-      <c r="N3" s="137"/>
-      <c r="O3" s="137"/>
-      <c r="P3" s="137"/>
-      <c r="Q3" s="137"/>
+      <c r="K3" s="137"/>
+      <c r="L3" s="137"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="139"/>
+      <c r="O3" s="139"/>
+      <c r="P3" s="139"/>
+      <c r="Q3" s="139"/>
     </row>
     <row r="4" spans="2:17">
-      <c r="B4" s="130" t="s">
+      <c r="B4" s="140" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="130"/>
-      <c r="D4" s="130"/>
-      <c r="E4" s="131"/>
-      <c r="F4" s="24" t="s">
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="141"/>
+      <c r="F4" s="92" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24" t="s">
+      <c r="G4" s="92"/>
+      <c r="H4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="61"/>
-      <c r="N4" s="94"/>
-      <c r="O4" s="94"/>
-      <c r="P4" s="94"/>
-      <c r="Q4" s="94"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="92"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="142"/>
+      <c r="O4" s="142"/>
+      <c r="P4" s="142"/>
+      <c r="Q4" s="142"/>
     </row>
     <row r="5" spans="2:17">
-      <c r="B5" s="130" t="s">
+      <c r="B5" s="140" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="130"/>
-      <c r="D5" s="130"/>
-      <c r="E5" s="131"/>
-      <c r="F5" s="24" t="s">
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="141"/>
+      <c r="F5" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="24"/>
-      <c r="I5" s="24"/>
-      <c r="J5" s="24" t="s">
+      <c r="G5" s="92"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="24"/>
-      <c r="L5" s="24"/>
-      <c r="M5" s="61"/>
-      <c r="N5" s="94"/>
-      <c r="O5" s="94"/>
-      <c r="P5" s="94"/>
-      <c r="Q5" s="94"/>
+      <c r="K5" s="92"/>
+      <c r="L5" s="92"/>
+      <c r="M5" s="95"/>
+      <c r="N5" s="142"/>
+      <c r="O5" s="142"/>
+      <c r="P5" s="142"/>
+      <c r="Q5" s="142"/>
     </row>
     <row r="6" spans="2:17">
-      <c r="B6" s="130" t="s">
+      <c r="B6" s="140" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="130"/>
-      <c r="D6" s="130"/>
-      <c r="E6" s="131"/>
-      <c r="F6" s="24" t="s">
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="141"/>
+      <c r="F6" s="92" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="61"/>
-      <c r="J6" s="23" t="s">
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="95"/>
+      <c r="J6" s="93" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="61"/>
-      <c r="N6" s="94"/>
-      <c r="O6" s="94"/>
-      <c r="P6" s="94"/>
-      <c r="Q6" s="94"/>
+      <c r="K6" s="92"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="142"/>
+      <c r="O6" s="142"/>
+      <c r="P6" s="142"/>
+      <c r="Q6" s="142"/>
     </row>
     <row r="7" spans="2:17">
-      <c r="B7" s="130" t="s">
+      <c r="B7" s="140" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="130"/>
-      <c r="D7" s="130"/>
-      <c r="E7" s="131"/>
-      <c r="F7" s="24" t="s">
+      <c r="C7" s="140"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="141"/>
+      <c r="F7" s="92" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="23" t="s">
+      <c r="G7" s="92"/>
+      <c r="H7" s="92"/>
+      <c r="I7" s="95"/>
+      <c r="J7" s="93" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="24"/>
-      <c r="L7" s="24"/>
-      <c r="M7" s="61"/>
-      <c r="N7" s="94"/>
-      <c r="O7" s="94"/>
-      <c r="P7" s="94"/>
-      <c r="Q7" s="94"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="92"/>
+      <c r="M7" s="95"/>
+      <c r="N7" s="142"/>
+      <c r="O7" s="142"/>
+      <c r="P7" s="142"/>
+      <c r="Q7" s="142"/>
     </row>
     <row r="8" spans="2:17">
-      <c r="B8" s="130" t="s">
+      <c r="B8" s="140" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="130"/>
-      <c r="D8" s="130"/>
-      <c r="E8" s="131"/>
-      <c r="F8" s="24" t="s">
+      <c r="C8" s="140"/>
+      <c r="D8" s="140"/>
+      <c r="E8" s="141"/>
+      <c r="F8" s="92" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="24"/>
-      <c r="H8" s="24"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24" t="s">
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="92"/>
+      <c r="J8" s="92" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="61"/>
-      <c r="N8" s="94"/>
-      <c r="O8" s="94"/>
-      <c r="P8" s="94"/>
-      <c r="Q8" s="94"/>
+      <c r="K8" s="92"/>
+      <c r="L8" s="92"/>
+      <c r="M8" s="95"/>
+      <c r="N8" s="142"/>
+      <c r="O8" s="142"/>
+      <c r="P8" s="142"/>
+      <c r="Q8" s="142"/>
     </row>
     <row r="9" spans="2:17">
-      <c r="B9" s="130" t="s">
+      <c r="B9" s="140" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="130"/>
-      <c r="D9" s="130"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="24" t="s">
+      <c r="C9" s="140"/>
+      <c r="D9" s="140"/>
+      <c r="E9" s="141"/>
+      <c r="F9" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24" t="s">
+      <c r="G9" s="92"/>
+      <c r="H9" s="92" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="61"/>
-      <c r="J9" s="23" t="s">
+      <c r="I9" s="95"/>
+      <c r="J9" s="93" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24">
+      <c r="K9" s="92"/>
+      <c r="L9" s="92">
         <v>2.5</v>
       </c>
-      <c r="M9" s="61"/>
-      <c r="N9" s="94"/>
-      <c r="O9" s="94"/>
-      <c r="P9" s="94"/>
-      <c r="Q9" s="94"/>
+      <c r="M9" s="95"/>
+      <c r="N9" s="142"/>
+      <c r="O9" s="142"/>
+      <c r="P9" s="142"/>
+      <c r="Q9" s="142"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:M2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="N3:Q3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="F4:I4"/>
-    <mergeCell ref="J4:M4"/>
-    <mergeCell ref="N4:Q4"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="F5:I5"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="F6:I6"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="N6:Q6"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="F7:I7"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="N7:Q7"/>
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="J8:M8"/>
@@ -6087,6 +6226,29 @@
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
     <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="F6:I6"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="J4:M4"/>
+    <mergeCell ref="N4:Q4"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="F5:I5"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:M2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:I3"/>
+    <mergeCell ref="J3:M3"/>
+    <mergeCell ref="N3:Q3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Poprawa działania algorytmu wyszukującego materiał pasujący do pozycji z boma. Poprawa wzorów kart kontroli łożysk garnkowych.
</commit_message>
<xml_diff>
--- a/data/wzor_PF.xlsx
+++ b/data/wzor_PF.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="2" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Arkusz1!$A$1:$R$56</definedName>
     <definedName name="Wybór1" localSheetId="0">Arkusz1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
   <si>
     <t>WYMIAR KONTROLNY</t>
   </si>
@@ -505,11 +505,14 @@
   <si>
     <t>TWARDOŚĆ: Sh⁰A 50 +/-5</t>
   </si>
+  <si>
+    <t>N.D.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;zł&quot;_-;\-* #,##0.00\ &quot;zł&quot;_-;_-* &quot;-&quot;??\ &quot;zł&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
@@ -1029,51 +1032,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1513,6 +1471,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2634,7 +2625,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2667,7 +2658,7 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2678,19 +2669,19 @@
     <xf numFmtId="0" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="29" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="29" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2703,64 +2694,64 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="40" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="31" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="31" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="31" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2772,24 +2763,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="30" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2799,7 +2826,7 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2811,207 +2838,207 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3021,7 +3048,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3038,42 +3065,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1101">
@@ -4273,16 +4264,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>209551</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>183047</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>70141</xdr:rowOff>
+      <xdr:rowOff>56888</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>169815</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>412942</xdr:colOff>
       <xdr:row>55</xdr:row>
-      <xdr:rowOff>138481</xdr:rowOff>
+      <xdr:rowOff>125228</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4299,8 +4290,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="567105" y="8399387"/>
-          <a:ext cx="2038351" cy="947570"/>
+          <a:off x="1084195" y="8438888"/>
+          <a:ext cx="2032190" cy="929731"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4312,13 +4303,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>114592</xdr:colOff>
+      <xdr:colOff>187479</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>70273</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>109074</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>105761</xdr:colOff>
       <xdr:row>55</xdr:row>
       <xdr:rowOff>38833</xdr:rowOff>
     </xdr:to>
@@ -4337,8 +4328,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4047684" y="8399519"/>
-          <a:ext cx="1726223" cy="847790"/>
+          <a:off x="5143792" y="8452273"/>
+          <a:ext cx="1720578" cy="829951"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4349,16 +4340,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>164124</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>158262</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>52755</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>11724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>272424</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>146003</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>383793</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>3797</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4369,7 +4360,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -4380,8 +4371,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="521678" y="1178170"/>
-          <a:ext cx="5303520" cy="2027555"/>
+          <a:off x="1406770" y="1406770"/>
+          <a:ext cx="5295761" cy="2027556"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4471,47 +4462,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor>
-        <xdr:from>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>114300</xdr:colOff>
-          <xdr:row>24</xdr:row>
-          <xdr:rowOff>76200</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>13</xdr:col>
-          <xdr:colOff>409575</xdr:colOff>
-          <xdr:row>25</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1025" name="Object 1" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1025"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
@@ -4590,7 +4540,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -4625,7 +4574,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Pakiet Office">
@@ -4801,46 +4749,46 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A13" zoomScale="130" zoomScaleNormal="70" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30:M32"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A40" zoomScale="115" zoomScaleNormal="70" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="O59" sqref="O59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="6.8984375" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="18" width="4.375" customWidth="1"/>
-    <col min="19" max="19" width="4.25" customWidth="1"/>
-    <col min="20" max="20" width="4.125" customWidth="1"/>
+    <col min="1" max="18" width="5.796875" customWidth="1"/>
+    <col min="19" max="19" width="4.19921875" customWidth="1"/>
+    <col min="20" max="20" width="4.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A2" s="98" t="s">
+    <row r="2" spans="1:18" ht="13.2" customHeight="1">
+      <c r="A2" s="111" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
-      <c r="J2" s="98"/>
-      <c r="K2" s="98"/>
-      <c r="L2" s="98"/>
-      <c r="M2" s="98"/>
-      <c r="N2" s="98"/>
-      <c r="O2" s="98"/>
-      <c r="P2" s="98"/>
-      <c r="Q2" s="98"/>
-      <c r="R2" s="98"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
+      <c r="R2" s="111"/>
     </row>
-    <row r="3" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
+    <row r="3" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -4860,66 +4808,66 @@
       <c r="Q3" s="21"/>
       <c r="R3" s="21"/>
     </row>
-    <row r="4" spans="1:18" ht="13.15" customHeight="1" thickTop="1">
-      <c r="A4" s="105" t="s">
+    <row r="4" spans="1:18" ht="13.2" customHeight="1" thickTop="1">
+      <c r="A4" s="118" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106" t="s">
+      <c r="B4" s="119"/>
+      <c r="C4" s="119" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106" t="s">
+      <c r="D4" s="119"/>
+      <c r="E4" s="119" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106" t="s">
+      <c r="F4" s="119"/>
+      <c r="G4" s="119" t="s">
         <v>72</v>
       </c>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106" t="s">
+      <c r="H4" s="119"/>
+      <c r="I4" s="119" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="106"/>
-      <c r="K4" s="106" t="s">
+      <c r="J4" s="119"/>
+      <c r="K4" s="119" t="s">
         <v>74</v>
       </c>
-      <c r="L4" s="106"/>
-      <c r="M4" s="106" t="s">
+      <c r="L4" s="119"/>
+      <c r="M4" s="119" t="s">
         <v>75</v>
       </c>
-      <c r="N4" s="106"/>
-      <c r="O4" s="106" t="s">
+      <c r="N4" s="119"/>
+      <c r="O4" s="119" t="s">
         <v>76</v>
       </c>
-      <c r="P4" s="106"/>
-      <c r="Q4" s="106" t="s">
+      <c r="P4" s="119"/>
+      <c r="Q4" s="119" t="s">
         <v>77</v>
       </c>
-      <c r="R4" s="109"/>
+      <c r="R4" s="122"/>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A5" s="107"/>
-      <c r="B5" s="108"/>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="108"/>
-      <c r="G5" s="108"/>
-      <c r="H5" s="108"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="108"/>
-      <c r="K5" s="108"/>
-      <c r="L5" s="108"/>
-      <c r="M5" s="108"/>
-      <c r="N5" s="108"/>
-      <c r="O5" s="108"/>
-      <c r="P5" s="108"/>
-      <c r="Q5" s="108"/>
-      <c r="R5" s="110"/>
+      <c r="A5" s="120"/>
+      <c r="B5" s="121"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="121"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="121"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="121"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="121"/>
+      <c r="K5" s="121"/>
+      <c r="L5" s="121"/>
+      <c r="M5" s="121"/>
+      <c r="N5" s="121"/>
+      <c r="O5" s="121"/>
+      <c r="P5" s="121"/>
+      <c r="Q5" s="121"/>
+      <c r="R5" s="123"/>
     </row>
-    <row r="6" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A6" s="111"/>
+    <row r="6" spans="1:18" ht="13.2" customHeight="1">
+      <c r="A6" s="124"/>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
       <c r="D6" s="23"/>
@@ -4938,8 +4886,8 @@
       <c r="Q6" s="23"/>
       <c r="R6" s="25"/>
     </row>
-    <row r="7" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
-      <c r="A7" s="112"/>
+    <row r="7" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
+      <c r="A7" s="125"/>
       <c r="B7" s="24"/>
       <c r="C7" s="24"/>
       <c r="D7" s="24"/>
@@ -4958,7 +4906,7 @@
       <c r="Q7" s="24"/>
       <c r="R7" s="26"/>
     </row>
-    <row r="8" spans="1:18" ht="13.15" customHeight="1" thickTop="1">
+    <row r="8" spans="1:18" ht="13.2" customHeight="1" thickTop="1">
       <c r="A8" s="18"/>
       <c r="B8" s="18"/>
       <c r="C8" s="18"/>
@@ -4978,32 +4926,32 @@
       <c r="Q8" s="18"/>
       <c r="R8" s="18"/>
     </row>
-    <row r="9" spans="1:18" ht="13.15" customHeight="1">
+    <row r="9" spans="1:18" ht="13.2" customHeight="1">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="13.15" customHeight="1">
+    <row r="10" spans="1:18" ht="13.2" customHeight="1">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="13.15" customHeight="1">
+    <row r="11" spans="1:18" ht="13.2" customHeight="1">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="13.15" customHeight="1">
+    <row r="12" spans="1:18" ht="13.2" customHeight="1">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="13.15" customHeight="1">
+    <row r="13" spans="1:18" ht="13.2" customHeight="1">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="13.15" customHeight="1">
+    <row r="14" spans="1:18" ht="13.2" customHeight="1">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:18" ht="13.15" customHeight="1">
+    <row r="15" spans="1:18" ht="13.2" customHeight="1">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:18" ht="13.15" customHeight="1"/>
-    <row r="17" spans="1:18" ht="13.15" customHeight="1"/>
-    <row r="18" spans="1:18" ht="13.15" customHeight="1"/>
-    <row r="19" spans="1:18" ht="13.15" customHeight="1"/>
-    <row r="20" spans="1:18" s="5" customFormat="1" ht="13.15" customHeight="1">
+    <row r="16" spans="1:18" ht="13.2" customHeight="1"/>
+    <row r="17" spans="1:18" ht="13.2" customHeight="1"/>
+    <row r="18" spans="1:18" ht="13.2" customHeight="1"/>
+    <row r="19" spans="1:18" ht="13.2" customHeight="1"/>
+    <row r="20" spans="1:18" s="5" customFormat="1" ht="13.2" customHeight="1">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
       <c r="C20" s="7"/>
@@ -5023,7 +4971,7 @@
       <c r="Q20"/>
       <c r="R20"/>
     </row>
-    <row r="21" spans="1:18" s="5" customFormat="1" ht="13.15" customHeight="1">
+    <row r="21" spans="1:18" s="5" customFormat="1" ht="13.2" customHeight="1">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
       <c r="C21" s="7"/>
@@ -5043,7 +4991,7 @@
       <c r="Q21"/>
       <c r="R21"/>
     </row>
-    <row r="22" spans="1:18" s="5" customFormat="1" ht="13.15" customHeight="1">
+    <row r="22" spans="1:18" s="5" customFormat="1" ht="13.2" customHeight="1">
       <c r="A22" s="11"/>
       <c r="B22" s="11"/>
       <c r="C22" s="8"/>
@@ -5054,7 +5002,7 @@
       <c r="H22" s="8"/>
       <c r="I22" s="9"/>
     </row>
-    <row r="23" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
+    <row r="23" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
       <c r="A23" s="27" t="s">
         <v>0</v>
       </c>
@@ -5104,7 +5052,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="13.15" customHeight="1">
+    <row r="24" spans="1:18" ht="13.2" customHeight="1">
       <c r="A24" s="29" t="s">
         <v>23</v>
       </c>
@@ -5142,7 +5090,7 @@
       </c>
       <c r="R24" s="12"/>
     </row>
-    <row r="25" spans="1:18" ht="13.15" customHeight="1">
+    <row r="25" spans="1:18" ht="13.2" customHeight="1">
       <c r="A25" s="31" t="s">
         <v>24</v>
       </c>
@@ -5174,17 +5122,17 @@
       <c r="O25" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="P25" s="58" t="s">
+      <c r="P25" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="Q25" s="58" t="s">
+      <c r="Q25" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="R25" s="59" t="s">
+      <c r="R25" s="70" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="13.15" customHeight="1">
+    <row r="26" spans="1:18" ht="13.2" customHeight="1">
       <c r="A26" s="34"/>
       <c r="B26" s="35"/>
       <c r="C26" s="35"/>
@@ -5204,31 +5152,31 @@
       <c r="M26" s="48"/>
       <c r="N26" s="49"/>
       <c r="O26" s="51"/>
-      <c r="P26" s="58"/>
-      <c r="Q26" s="58"/>
-      <c r="R26" s="59"/>
+      <c r="P26" s="69"/>
+      <c r="Q26" s="69"/>
+      <c r="R26" s="70"/>
     </row>
-    <row r="27" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A27" s="54" t="s">
+    <row r="27" spans="1:18" ht="13.2" customHeight="1">
+      <c r="A27" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="54"/>
-      <c r="C27" s="54"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
       <c r="J27" s="53"/>
       <c r="K27" s="53"/>
-      <c r="L27" s="63" t="s">
+      <c r="L27" s="75" t="s">
         <v>80</v>
       </c>
-      <c r="M27" s="63" t="s">
+      <c r="M27" s="75" t="s">
         <v>80</v>
       </c>
-      <c r="N27" s="63" t="s">
+      <c r="N27" s="75" t="s">
         <v>80</v>
       </c>
       <c r="O27" s="53" t="s">
@@ -5242,179 +5190,181 @@
       </c>
       <c r="R27" s="53"/>
     </row>
-    <row r="28" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A28" s="54"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="61"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="62"/>
+    <row r="28" spans="1:18" ht="13.2" customHeight="1">
+      <c r="A28" s="71"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="72"/>
+      <c r="E28" s="73"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
       <c r="J28" s="53"/>
       <c r="K28" s="53"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="64"/>
-      <c r="N28" s="64"/>
+      <c r="L28" s="76"/>
+      <c r="M28" s="76"/>
+      <c r="N28" s="76"/>
       <c r="O28" s="53"/>
       <c r="P28" s="53"/>
       <c r="Q28" s="53"/>
       <c r="R28" s="53"/>
     </row>
-    <row r="29" spans="1:18" ht="13.15" customHeight="1"/>
-    <row r="30" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A30" s="54" t="s">
+    <row r="29" spans="1:18" ht="13.2" customHeight="1"/>
+    <row r="30" spans="1:18" ht="13.2" customHeight="1">
+      <c r="A30" s="71" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="54"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="143" t="s">
+      <c r="B30" s="71"/>
+      <c r="C30" s="72"/>
+      <c r="D30" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="E30" s="144"/>
-      <c r="F30" s="144"/>
-      <c r="G30" s="144"/>
-      <c r="H30" s="145"/>
-      <c r="I30" s="152" t="s">
+      <c r="E30" s="55"/>
+      <c r="F30" s="55"/>
+      <c r="G30" s="55"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="J30" s="144"/>
-      <c r="K30" s="144"/>
-      <c r="L30" s="144"/>
-      <c r="M30" s="145"/>
-      <c r="N30" s="55" t="s">
+      <c r="J30" s="55"/>
+      <c r="K30" s="55"/>
+      <c r="L30" s="55"/>
+      <c r="M30" s="56"/>
+      <c r="N30" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="O30" s="56"/>
-      <c r="P30" s="56"/>
-      <c r="Q30" s="56"/>
-      <c r="R30" s="56"/>
+      <c r="O30" s="67"/>
+      <c r="P30" s="67"/>
+      <c r="Q30" s="67"/>
+      <c r="R30" s="67"/>
     </row>
-    <row r="31" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A31" s="54"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="146"/>
-      <c r="E31" s="147"/>
-      <c r="F31" s="147"/>
-      <c r="G31" s="147"/>
-      <c r="H31" s="148"/>
-      <c r="I31" s="153"/>
-      <c r="J31" s="147"/>
-      <c r="K31" s="147"/>
-      <c r="L31" s="147"/>
-      <c r="M31" s="148"/>
-      <c r="N31" s="56"/>
-      <c r="O31" s="56"/>
-      <c r="P31" s="56"/>
-      <c r="Q31" s="56"/>
-      <c r="R31" s="56"/>
+    <row r="31" spans="1:18" ht="13.2" customHeight="1">
+      <c r="A31" s="71"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="72"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="64"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="67"/>
+      <c r="O31" s="67"/>
+      <c r="P31" s="67"/>
+      <c r="Q31" s="67"/>
+      <c r="R31" s="67"/>
     </row>
-    <row r="32" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
+    <row r="32" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
       <c r="A32" s="27"/>
       <c r="B32" s="27"/>
       <c r="C32" s="28"/>
-      <c r="D32" s="149"/>
-      <c r="E32" s="150"/>
-      <c r="F32" s="150"/>
-      <c r="G32" s="150"/>
-      <c r="H32" s="151"/>
-      <c r="I32" s="154"/>
-      <c r="J32" s="150"/>
-      <c r="K32" s="150"/>
-      <c r="L32" s="150"/>
-      <c r="M32" s="151"/>
-      <c r="N32" s="57"/>
-      <c r="O32" s="57"/>
-      <c r="P32" s="57"/>
-      <c r="Q32" s="57"/>
-      <c r="R32" s="57"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="62"/>
+      <c r="N32" s="68"/>
+      <c r="O32" s="68"/>
+      <c r="P32" s="68"/>
+      <c r="Q32" s="68"/>
+      <c r="R32" s="68"/>
     </row>
-    <row r="33" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
-      <c r="A33" s="81" t="s">
+    <row r="33" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
+      <c r="A33" s="93" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="81"/>
-      <c r="C33" s="82"/>
-      <c r="D33" s="83" t="s">
+      <c r="B33" s="93"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="E33" s="84"/>
-      <c r="F33" s="84"/>
-      <c r="G33" s="85"/>
-      <c r="H33" s="85"/>
-      <c r="I33" s="84" t="s">
+      <c r="E33" s="96"/>
+      <c r="F33" s="96"/>
+      <c r="G33" s="97"/>
+      <c r="H33" s="97"/>
+      <c r="I33" s="96" t="s">
         <v>39</v>
       </c>
-      <c r="J33" s="84"/>
-      <c r="K33" s="84"/>
-      <c r="L33" s="85"/>
-      <c r="M33" s="85"/>
-      <c r="N33" s="65" t="s">
+      <c r="J33" s="96"/>
+      <c r="K33" s="96"/>
+      <c r="L33" s="97"/>
+      <c r="M33" s="97"/>
+      <c r="N33" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="O33" s="65"/>
-      <c r="P33" s="65"/>
-      <c r="Q33" s="66"/>
-      <c r="R33" s="66"/>
+      <c r="O33" s="77"/>
+      <c r="P33" s="77"/>
+      <c r="Q33" s="78"/>
+      <c r="R33" s="78"/>
     </row>
-    <row r="34" spans="1:18" ht="13.15" customHeight="1">
-      <c r="A34" s="67" t="s">
+    <row r="34" spans="1:18" ht="13.2" customHeight="1">
+      <c r="A34" s="79" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="68"/>
-      <c r="C34" s="69"/>
-      <c r="D34" s="68" t="s">
+      <c r="B34" s="80"/>
+      <c r="C34" s="81"/>
+      <c r="D34" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="68"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="74"/>
-      <c r="I34" s="68" t="s">
+      <c r="E34" s="80"/>
+      <c r="F34" s="80"/>
+      <c r="G34" s="85" t="s">
+        <v>82</v>
+      </c>
+      <c r="H34" s="86"/>
+      <c r="I34" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="J34" s="68"/>
-      <c r="K34" s="68"/>
-      <c r="L34" s="77"/>
-      <c r="M34" s="78"/>
-      <c r="N34" s="68" t="s">
+      <c r="J34" s="80"/>
+      <c r="K34" s="80"/>
+      <c r="L34" s="89"/>
+      <c r="M34" s="90"/>
+      <c r="N34" s="80" t="s">
         <v>42</v>
       </c>
-      <c r="O34" s="68"/>
-      <c r="P34" s="68"/>
-      <c r="Q34" s="77"/>
-      <c r="R34" s="78"/>
+      <c r="O34" s="80"/>
+      <c r="P34" s="80"/>
+      <c r="Q34" s="89"/>
+      <c r="R34" s="90"/>
     </row>
-    <row r="35" spans="1:18" ht="13.15" customHeight="1" thickBot="1">
-      <c r="A35" s="70"/>
-      <c r="B35" s="71"/>
-      <c r="C35" s="72"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="71"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="71"/>
-      <c r="K35" s="71"/>
-      <c r="L35" s="79"/>
-      <c r="M35" s="80"/>
-      <c r="N35" s="71"/>
-      <c r="O35" s="71"/>
-      <c r="P35" s="71"/>
-      <c r="Q35" s="79"/>
-      <c r="R35" s="80"/>
+    <row r="35" spans="1:18" ht="13.2" customHeight="1" thickBot="1">
+      <c r="A35" s="82"/>
+      <c r="B35" s="83"/>
+      <c r="C35" s="84"/>
+      <c r="D35" s="83"/>
+      <c r="E35" s="83"/>
+      <c r="F35" s="83"/>
+      <c r="G35" s="87"/>
+      <c r="H35" s="88"/>
+      <c r="I35" s="83"/>
+      <c r="J35" s="83"/>
+      <c r="K35" s="83"/>
+      <c r="L35" s="91"/>
+      <c r="M35" s="92"/>
+      <c r="N35" s="83"/>
+      <c r="O35" s="83"/>
+      <c r="P35" s="83"/>
+      <c r="Q35" s="91"/>
+      <c r="R35" s="92"/>
     </row>
-    <row r="37" spans="1:18" ht="15" thickBot="1">
-      <c r="A37" s="132" t="s">
+    <row r="37" spans="1:18" ht="14.4" thickBot="1">
+      <c r="A37" s="135" t="s">
         <v>7</v>
       </c>
-      <c r="B37" s="124"/>
-      <c r="C37" s="124"/>
-      <c r="D37" s="124"/>
-      <c r="E37" s="133"/>
+      <c r="B37" s="136"/>
+      <c r="C37" s="136"/>
+      <c r="D37" s="136"/>
+      <c r="E37" s="137"/>
       <c r="F37" s="22" t="s">
         <v>2</v>
       </c>
@@ -5425,435 +5375,441 @@
       <c r="K37" s="22"/>
       <c r="L37" s="22"/>
       <c r="M37" s="22"/>
-      <c r="N37" s="123" t="s">
+      <c r="N37" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="O37" s="124"/>
-      <c r="P37" s="124"/>
-      <c r="Q37" s="124"/>
-      <c r="R37" s="125"/>
+      <c r="O37" s="136"/>
+      <c r="P37" s="136"/>
+      <c r="Q37" s="136"/>
+      <c r="R37" s="139"/>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="96" t="s">
+      <c r="A38" s="108" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="94"/>
-      <c r="C38" s="94"/>
-      <c r="D38" s="94"/>
-      <c r="E38" s="97"/>
-      <c r="F38" s="94" t="s">
+      <c r="B38" s="106"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="109"/>
+      <c r="F38" s="106" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="94"/>
-      <c r="H38" s="94"/>
-      <c r="I38" s="94"/>
-      <c r="J38" s="94" t="s">
+      <c r="G38" s="106"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="106" t="s">
         <v>56</v>
       </c>
-      <c r="K38" s="94"/>
-      <c r="L38" s="94"/>
-      <c r="M38" s="94"/>
-      <c r="N38" s="126"/>
-      <c r="O38" s="127"/>
-      <c r="P38" s="127"/>
-      <c r="Q38" s="127"/>
-      <c r="R38" s="128"/>
+      <c r="K38" s="106"/>
+      <c r="L38" s="106"/>
+      <c r="M38" s="106"/>
+      <c r="N38" s="140"/>
+      <c r="O38" s="141"/>
+      <c r="P38" s="141"/>
+      <c r="Q38" s="141"/>
+      <c r="R38" s="142"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="93" t="s">
+      <c r="A39" s="105" t="s">
         <v>43</v>
       </c>
-      <c r="B39" s="92"/>
-      <c r="C39" s="92"/>
-      <c r="D39" s="92"/>
-      <c r="E39" s="122"/>
-      <c r="F39" s="92" t="s">
+      <c r="B39" s="104"/>
+      <c r="C39" s="104"/>
+      <c r="D39" s="104"/>
+      <c r="E39" s="110"/>
+      <c r="F39" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="G39" s="92"/>
-      <c r="H39" s="92"/>
-      <c r="I39" s="92"/>
-      <c r="J39" s="92" t="s">
+      <c r="G39" s="104"/>
+      <c r="H39" s="104"/>
+      <c r="I39" s="104"/>
+      <c r="J39" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="K39" s="92"/>
-      <c r="L39" s="92"/>
-      <c r="M39" s="92"/>
-      <c r="N39" s="129"/>
-      <c r="O39" s="130"/>
-      <c r="P39" s="130"/>
-      <c r="Q39" s="130"/>
-      <c r="R39" s="131"/>
+      <c r="K39" s="104"/>
+      <c r="L39" s="104"/>
+      <c r="M39" s="104"/>
+      <c r="N39" s="143"/>
+      <c r="O39" s="144"/>
+      <c r="P39" s="144"/>
+      <c r="Q39" s="144"/>
+      <c r="R39" s="145"/>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="93" t="s">
+      <c r="A40" s="105" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="92"/>
-      <c r="C40" s="92"/>
-      <c r="D40" s="92"/>
-      <c r="E40" s="122"/>
-      <c r="F40" s="92" t="s">
+      <c r="B40" s="104"/>
+      <c r="C40" s="104"/>
+      <c r="D40" s="104"/>
+      <c r="E40" s="110"/>
+      <c r="F40" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="G40" s="92"/>
-      <c r="H40" s="92"/>
-      <c r="I40" s="92"/>
-      <c r="J40" s="92" t="s">
+      <c r="G40" s="104"/>
+      <c r="H40" s="104"/>
+      <c r="I40" s="104"/>
+      <c r="J40" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="K40" s="92"/>
-      <c r="L40" s="92"/>
-      <c r="M40" s="92"/>
-      <c r="N40" s="129"/>
-      <c r="O40" s="130"/>
-      <c r="P40" s="130"/>
-      <c r="Q40" s="130"/>
-      <c r="R40" s="131"/>
+      <c r="K40" s="104"/>
+      <c r="L40" s="104"/>
+      <c r="M40" s="104"/>
+      <c r="N40" s="143" t="s">
+        <v>82</v>
+      </c>
+      <c r="O40" s="144"/>
+      <c r="P40" s="144"/>
+      <c r="Q40" s="144"/>
+      <c r="R40" s="145"/>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="93" t="s">
+      <c r="A41" s="105" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="92"/>
-      <c r="C41" s="92"/>
-      <c r="D41" s="92"/>
-      <c r="E41" s="122"/>
-      <c r="F41" s="92" t="s">
+      <c r="B41" s="104"/>
+      <c r="C41" s="104"/>
+      <c r="D41" s="104"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="G41" s="92"/>
-      <c r="H41" s="92"/>
-      <c r="I41" s="95"/>
-      <c r="J41" s="93" t="s">
+      <c r="G41" s="104"/>
+      <c r="H41" s="104"/>
+      <c r="I41" s="107"/>
+      <c r="J41" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="K41" s="92"/>
-      <c r="L41" s="92"/>
-      <c r="M41" s="92"/>
-      <c r="N41" s="129"/>
-      <c r="O41" s="130"/>
-      <c r="P41" s="130"/>
-      <c r="Q41" s="130"/>
-      <c r="R41" s="131"/>
+      <c r="K41" s="104"/>
+      <c r="L41" s="104"/>
+      <c r="M41" s="104"/>
+      <c r="N41" s="143" t="s">
+        <v>82</v>
+      </c>
+      <c r="O41" s="144"/>
+      <c r="P41" s="144"/>
+      <c r="Q41" s="144"/>
+      <c r="R41" s="145"/>
     </row>
     <row r="42" spans="1:18">
-      <c r="A42" s="93" t="s">
+      <c r="A42" s="105" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="92"/>
-      <c r="C42" s="92"/>
-      <c r="D42" s="92"/>
-      <c r="E42" s="122"/>
-      <c r="F42" s="92" t="s">
+      <c r="B42" s="104"/>
+      <c r="C42" s="104"/>
+      <c r="D42" s="104"/>
+      <c r="E42" s="110"/>
+      <c r="F42" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="G42" s="92"/>
-      <c r="H42" s="92"/>
-      <c r="I42" s="95"/>
-      <c r="J42" s="93" t="s">
+      <c r="G42" s="104"/>
+      <c r="H42" s="104"/>
+      <c r="I42" s="107"/>
+      <c r="J42" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="K42" s="92"/>
-      <c r="L42" s="92"/>
-      <c r="M42" s="92"/>
-      <c r="N42" s="129"/>
-      <c r="O42" s="130"/>
-      <c r="P42" s="130"/>
-      <c r="Q42" s="130"/>
-      <c r="R42" s="131"/>
+      <c r="K42" s="104"/>
+      <c r="L42" s="104"/>
+      <c r="M42" s="104"/>
+      <c r="N42" s="143"/>
+      <c r="O42" s="144"/>
+      <c r="P42" s="144"/>
+      <c r="Q42" s="144"/>
+      <c r="R42" s="145"/>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="93" t="s">
+      <c r="A43" s="105" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="92"/>
-      <c r="C43" s="92"/>
-      <c r="D43" s="92"/>
-      <c r="E43" s="122"/>
-      <c r="F43" s="92" t="s">
+      <c r="B43" s="104"/>
+      <c r="C43" s="104"/>
+      <c r="D43" s="104"/>
+      <c r="E43" s="110"/>
+      <c r="F43" s="104" t="s">
         <v>53</v>
       </c>
-      <c r="G43" s="92"/>
-      <c r="H43" s="92"/>
-      <c r="I43" s="92"/>
-      <c r="J43" s="92" t="s">
+      <c r="G43" s="104"/>
+      <c r="H43" s="104"/>
+      <c r="I43" s="104"/>
+      <c r="J43" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="K43" s="92"/>
-      <c r="L43" s="92"/>
-      <c r="M43" s="92"/>
-      <c r="N43" s="129"/>
-      <c r="O43" s="130"/>
-      <c r="P43" s="130"/>
-      <c r="Q43" s="130"/>
-      <c r="R43" s="131"/>
+      <c r="K43" s="104"/>
+      <c r="L43" s="104"/>
+      <c r="M43" s="104"/>
+      <c r="N43" s="143"/>
+      <c r="O43" s="144"/>
+      <c r="P43" s="144"/>
+      <c r="Q43" s="144"/>
+      <c r="R43" s="145"/>
     </row>
     <row r="44" spans="1:18">
-      <c r="A44" s="93" t="s">
+      <c r="A44" s="105" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="92"/>
-      <c r="C44" s="92"/>
-      <c r="D44" s="92"/>
-      <c r="E44" s="122"/>
-      <c r="F44" s="92" t="s">
+      <c r="B44" s="104"/>
+      <c r="C44" s="104"/>
+      <c r="D44" s="104"/>
+      <c r="E44" s="110"/>
+      <c r="F44" s="104" t="s">
         <v>54</v>
       </c>
-      <c r="G44" s="92"/>
-      <c r="H44" s="92" t="s">
+      <c r="G44" s="104"/>
+      <c r="H44" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="I44" s="95"/>
-      <c r="J44" s="93" t="s">
+      <c r="I44" s="107"/>
+      <c r="J44" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="K44" s="92"/>
-      <c r="L44" s="92">
+      <c r="K44" s="104"/>
+      <c r="L44" s="104">
         <v>2.5</v>
       </c>
-      <c r="M44" s="92"/>
-      <c r="N44" s="129"/>
-      <c r="O44" s="130"/>
-      <c r="P44" s="130"/>
-      <c r="Q44" s="130"/>
-      <c r="R44" s="131"/>
+      <c r="M44" s="104"/>
+      <c r="N44" s="143" t="s">
+        <v>82</v>
+      </c>
+      <c r="O44" s="144"/>
+      <c r="P44" s="144"/>
+      <c r="Q44" s="144"/>
+      <c r="R44" s="145"/>
     </row>
-    <row r="46" spans="1:18">
-      <c r="A46" s="117" t="s">
+    <row r="46" spans="1:18" ht="14.4">
+      <c r="A46" s="130" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="118"/>
-      <c r="C46" s="118"/>
-      <c r="D46" s="118"/>
-      <c r="E46" s="118"/>
-      <c r="F46" s="119"/>
+      <c r="B46" s="131"/>
+      <c r="C46" s="131"/>
+      <c r="D46" s="131"/>
+      <c r="E46" s="131"/>
+      <c r="F46" s="132"/>
       <c r="G46" s="17"/>
-      <c r="H46" s="120" t="s">
+      <c r="H46" s="133" t="s">
         <v>63</v>
       </c>
-      <c r="I46" s="120"/>
-      <c r="J46" s="120"/>
-      <c r="K46" s="120"/>
-      <c r="L46" s="121"/>
+      <c r="I46" s="133"/>
+      <c r="J46" s="133"/>
+      <c r="K46" s="133"/>
+      <c r="L46" s="134"/>
       <c r="M46" s="17"/>
-      <c r="N46" s="120" t="s">
+      <c r="N46" s="133" t="s">
         <v>64</v>
       </c>
-      <c r="O46" s="120"/>
-      <c r="P46" s="120"/>
-      <c r="Q46" s="120"/>
-      <c r="R46" s="121"/>
+      <c r="O46" s="133"/>
+      <c r="P46" s="133"/>
+      <c r="Q46" s="133"/>
+      <c r="R46" s="134"/>
     </row>
     <row r="47" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A47" s="113" t="s">
+      <c r="A47" s="126" t="s">
         <v>6</v>
       </c>
-      <c r="B47" s="114"/>
-      <c r="C47" s="115"/>
-      <c r="D47" s="115"/>
-      <c r="E47" s="115"/>
-      <c r="F47" s="115"/>
-      <c r="G47" s="115"/>
-      <c r="H47" s="115"/>
-      <c r="I47" s="115"/>
-      <c r="J47" s="115"/>
-      <c r="K47" s="115"/>
-      <c r="L47" s="115"/>
-      <c r="M47" s="115"/>
-      <c r="N47" s="115"/>
-      <c r="O47" s="115"/>
-      <c r="P47" s="115"/>
-      <c r="Q47" s="115"/>
-      <c r="R47" s="116"/>
+      <c r="B47" s="127"/>
+      <c r="C47" s="128"/>
+      <c r="D47" s="128"/>
+      <c r="E47" s="128"/>
+      <c r="F47" s="128"/>
+      <c r="G47" s="128"/>
+      <c r="H47" s="128"/>
+      <c r="I47" s="128"/>
+      <c r="J47" s="128"/>
+      <c r="K47" s="128"/>
+      <c r="L47" s="128"/>
+      <c r="M47" s="128"/>
+      <c r="N47" s="128"/>
+      <c r="O47" s="128"/>
+      <c r="P47" s="128"/>
+      <c r="Q47" s="128"/>
+      <c r="R47" s="129"/>
     </row>
     <row r="48" spans="1:18" ht="11.25" customHeight="1">
-      <c r="A48" s="102"/>
-      <c r="B48" s="103"/>
-      <c r="C48" s="103"/>
-      <c r="D48" s="103"/>
-      <c r="E48" s="103"/>
-      <c r="F48" s="103"/>
-      <c r="G48" s="103"/>
-      <c r="H48" s="103"/>
-      <c r="I48" s="103"/>
-      <c r="J48" s="103"/>
-      <c r="K48" s="103"/>
-      <c r="L48" s="103"/>
-      <c r="M48" s="103"/>
-      <c r="N48" s="103"/>
-      <c r="O48" s="103"/>
-      <c r="P48" s="103"/>
-      <c r="Q48" s="103"/>
-      <c r="R48" s="104"/>
+      <c r="A48" s="115"/>
+      <c r="B48" s="116"/>
+      <c r="C48" s="116"/>
+      <c r="D48" s="116"/>
+      <c r="E48" s="116"/>
+      <c r="F48" s="116"/>
+      <c r="G48" s="116"/>
+      <c r="H48" s="116"/>
+      <c r="I48" s="116"/>
+      <c r="J48" s="116"/>
+      <c r="K48" s="116"/>
+      <c r="L48" s="116"/>
+      <c r="M48" s="116"/>
+      <c r="N48" s="116"/>
+      <c r="O48" s="116"/>
+      <c r="P48" s="116"/>
+      <c r="Q48" s="116"/>
+      <c r="R48" s="117"/>
     </row>
     <row r="49" spans="1:18">
-      <c r="A49" s="86" t="s">
+      <c r="A49" s="98" t="s">
         <v>65</v>
       </c>
-      <c r="B49" s="87"/>
-      <c r="C49" s="87"/>
-      <c r="D49" s="87"/>
-      <c r="E49" s="87"/>
-      <c r="F49" s="87"/>
-      <c r="G49" s="87"/>
-      <c r="H49" s="87"/>
-      <c r="I49" s="88"/>
-      <c r="J49" s="86" t="s">
+      <c r="B49" s="99"/>
+      <c r="C49" s="99"/>
+      <c r="D49" s="99"/>
+      <c r="E49" s="99"/>
+      <c r="F49" s="99"/>
+      <c r="G49" s="99"/>
+      <c r="H49" s="99"/>
+      <c r="I49" s="100"/>
+      <c r="J49" s="98" t="s">
         <v>67</v>
       </c>
-      <c r="K49" s="87"/>
-      <c r="L49" s="87"/>
-      <c r="M49" s="87"/>
-      <c r="N49" s="87"/>
-      <c r="O49" s="87"/>
-      <c r="P49" s="87"/>
-      <c r="Q49" s="87"/>
-      <c r="R49" s="88"/>
+      <c r="K49" s="99"/>
+      <c r="L49" s="99"/>
+      <c r="M49" s="99"/>
+      <c r="N49" s="99"/>
+      <c r="O49" s="99"/>
+      <c r="P49" s="99"/>
+      <c r="Q49" s="99"/>
+      <c r="R49" s="100"/>
     </row>
     <row r="50" spans="1:18">
-      <c r="A50" s="89" t="s">
+      <c r="A50" s="101" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="90"/>
-      <c r="C50" s="90"/>
-      <c r="D50" s="90"/>
-      <c r="E50" s="90"/>
-      <c r="F50" s="90"/>
-      <c r="G50" s="90"/>
-      <c r="H50" s="90"/>
-      <c r="I50" s="91"/>
-      <c r="J50" s="89" t="s">
+      <c r="B50" s="102"/>
+      <c r="C50" s="102"/>
+      <c r="D50" s="102"/>
+      <c r="E50" s="102"/>
+      <c r="F50" s="102"/>
+      <c r="G50" s="102"/>
+      <c r="H50" s="102"/>
+      <c r="I50" s="103"/>
+      <c r="J50" s="101" t="s">
         <v>68</v>
       </c>
-      <c r="K50" s="90"/>
-      <c r="L50" s="90"/>
-      <c r="M50" s="90"/>
-      <c r="N50" s="90"/>
-      <c r="O50" s="90"/>
-      <c r="P50" s="90"/>
-      <c r="Q50" s="90"/>
-      <c r="R50" s="91"/>
+      <c r="K50" s="102"/>
+      <c r="L50" s="102"/>
+      <c r="M50" s="102"/>
+      <c r="N50" s="102"/>
+      <c r="O50" s="102"/>
+      <c r="P50" s="102"/>
+      <c r="Q50" s="102"/>
+      <c r="R50" s="103"/>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="99"/>
-      <c r="B51" s="100"/>
-      <c r="C51" s="100"/>
-      <c r="D51" s="100"/>
-      <c r="E51" s="100"/>
-      <c r="F51" s="100"/>
-      <c r="G51" s="100"/>
-      <c r="H51" s="100"/>
-      <c r="I51" s="101"/>
-      <c r="J51" s="99"/>
-      <c r="K51" s="100"/>
-      <c r="L51" s="100"/>
-      <c r="M51" s="100"/>
-      <c r="N51" s="100"/>
-      <c r="O51" s="100"/>
-      <c r="P51" s="100"/>
-      <c r="Q51" s="100"/>
-      <c r="R51" s="101"/>
+      <c r="A51" s="112"/>
+      <c r="B51" s="113"/>
+      <c r="C51" s="113"/>
+      <c r="D51" s="113"/>
+      <c r="E51" s="113"/>
+      <c r="F51" s="113"/>
+      <c r="G51" s="113"/>
+      <c r="H51" s="113"/>
+      <c r="I51" s="114"/>
+      <c r="J51" s="112"/>
+      <c r="K51" s="113"/>
+      <c r="L51" s="113"/>
+      <c r="M51" s="113"/>
+      <c r="N51" s="113"/>
+      <c r="O51" s="113"/>
+      <c r="P51" s="113"/>
+      <c r="Q51" s="113"/>
+      <c r="R51" s="114"/>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="99"/>
-      <c r="B52" s="100"/>
-      <c r="C52" s="100"/>
-      <c r="D52" s="100"/>
-      <c r="E52" s="100"/>
-      <c r="F52" s="100"/>
-      <c r="G52" s="100"/>
-      <c r="H52" s="100"/>
-      <c r="I52" s="101"/>
-      <c r="J52" s="99"/>
-      <c r="K52" s="100"/>
-      <c r="L52" s="100"/>
-      <c r="M52" s="100"/>
-      <c r="N52" s="100"/>
-      <c r="O52" s="100"/>
-      <c r="P52" s="100"/>
-      <c r="Q52" s="100"/>
-      <c r="R52" s="101"/>
+      <c r="A52" s="112"/>
+      <c r="B52" s="113"/>
+      <c r="C52" s="113"/>
+      <c r="D52" s="113"/>
+      <c r="E52" s="113"/>
+      <c r="F52" s="113"/>
+      <c r="G52" s="113"/>
+      <c r="H52" s="113"/>
+      <c r="I52" s="114"/>
+      <c r="J52" s="112"/>
+      <c r="K52" s="113"/>
+      <c r="L52" s="113"/>
+      <c r="M52" s="113"/>
+      <c r="N52" s="113"/>
+      <c r="O52" s="113"/>
+      <c r="P52" s="113"/>
+      <c r="Q52" s="113"/>
+      <c r="R52" s="114"/>
     </row>
     <row r="53" spans="1:18">
-      <c r="A53" s="99"/>
-      <c r="B53" s="100"/>
-      <c r="C53" s="100"/>
-      <c r="D53" s="100"/>
-      <c r="E53" s="100"/>
-      <c r="F53" s="100"/>
-      <c r="G53" s="100"/>
-      <c r="H53" s="100"/>
-      <c r="I53" s="101"/>
-      <c r="J53" s="99"/>
-      <c r="K53" s="100"/>
-      <c r="L53" s="100"/>
-      <c r="M53" s="100"/>
-      <c r="N53" s="100"/>
-      <c r="O53" s="100"/>
-      <c r="P53" s="100"/>
-      <c r="Q53" s="100"/>
-      <c r="R53" s="101"/>
+      <c r="A53" s="112"/>
+      <c r="B53" s="113"/>
+      <c r="C53" s="113"/>
+      <c r="D53" s="113"/>
+      <c r="E53" s="113"/>
+      <c r="F53" s="113"/>
+      <c r="G53" s="113"/>
+      <c r="H53" s="113"/>
+      <c r="I53" s="114"/>
+      <c r="J53" s="112"/>
+      <c r="K53" s="113"/>
+      <c r="L53" s="113"/>
+      <c r="M53" s="113"/>
+      <c r="N53" s="113"/>
+      <c r="O53" s="113"/>
+      <c r="P53" s="113"/>
+      <c r="Q53" s="113"/>
+      <c r="R53" s="114"/>
     </row>
     <row r="54" spans="1:18">
-      <c r="A54" s="99"/>
-      <c r="B54" s="100"/>
-      <c r="C54" s="100"/>
-      <c r="D54" s="100"/>
-      <c r="E54" s="100"/>
-      <c r="F54" s="100"/>
-      <c r="G54" s="100"/>
-      <c r="H54" s="100"/>
-      <c r="I54" s="101"/>
-      <c r="J54" s="99"/>
-      <c r="K54" s="100"/>
-      <c r="L54" s="100"/>
-      <c r="M54" s="100"/>
-      <c r="N54" s="100"/>
-      <c r="O54" s="100"/>
-      <c r="P54" s="100"/>
-      <c r="Q54" s="100"/>
-      <c r="R54" s="101"/>
+      <c r="A54" s="112"/>
+      <c r="B54" s="113"/>
+      <c r="C54" s="113"/>
+      <c r="D54" s="113"/>
+      <c r="E54" s="113"/>
+      <c r="F54" s="113"/>
+      <c r="G54" s="113"/>
+      <c r="H54" s="113"/>
+      <c r="I54" s="114"/>
+      <c r="J54" s="112"/>
+      <c r="K54" s="113"/>
+      <c r="L54" s="113"/>
+      <c r="M54" s="113"/>
+      <c r="N54" s="113"/>
+      <c r="O54" s="113"/>
+      <c r="P54" s="113"/>
+      <c r="Q54" s="113"/>
+      <c r="R54" s="114"/>
     </row>
     <row r="55" spans="1:18">
-      <c r="A55" s="99"/>
-      <c r="B55" s="100"/>
-      <c r="C55" s="100"/>
-      <c r="D55" s="100"/>
-      <c r="E55" s="100"/>
-      <c r="F55" s="100"/>
-      <c r="G55" s="100"/>
-      <c r="H55" s="100"/>
-      <c r="I55" s="101"/>
-      <c r="J55" s="99"/>
-      <c r="K55" s="100"/>
-      <c r="L55" s="100"/>
-      <c r="M55" s="100"/>
-      <c r="N55" s="100"/>
-      <c r="O55" s="100"/>
-      <c r="P55" s="100"/>
-      <c r="Q55" s="100"/>
-      <c r="R55" s="101"/>
+      <c r="A55" s="112"/>
+      <c r="B55" s="113"/>
+      <c r="C55" s="113"/>
+      <c r="D55" s="113"/>
+      <c r="E55" s="113"/>
+      <c r="F55" s="113"/>
+      <c r="G55" s="113"/>
+      <c r="H55" s="113"/>
+      <c r="I55" s="114"/>
+      <c r="J55" s="112"/>
+      <c r="K55" s="113"/>
+      <c r="L55" s="113"/>
+      <c r="M55" s="113"/>
+      <c r="N55" s="113"/>
+      <c r="O55" s="113"/>
+      <c r="P55" s="113"/>
+      <c r="Q55" s="113"/>
+      <c r="R55" s="114"/>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" s="102"/>
-      <c r="B56" s="103"/>
-      <c r="C56" s="103"/>
-      <c r="D56" s="103"/>
-      <c r="E56" s="103"/>
-      <c r="F56" s="103"/>
-      <c r="G56" s="103"/>
-      <c r="H56" s="103"/>
-      <c r="I56" s="104"/>
-      <c r="J56" s="102"/>
-      <c r="K56" s="103"/>
-      <c r="L56" s="103"/>
-      <c r="M56" s="103"/>
-      <c r="N56" s="103"/>
-      <c r="O56" s="103"/>
-      <c r="P56" s="103"/>
-      <c r="Q56" s="103"/>
-      <c r="R56" s="104"/>
+      <c r="A56" s="115"/>
+      <c r="B56" s="116"/>
+      <c r="C56" s="116"/>
+      <c r="D56" s="116"/>
+      <c r="E56" s="116"/>
+      <c r="F56" s="116"/>
+      <c r="G56" s="116"/>
+      <c r="H56" s="116"/>
+      <c r="I56" s="117"/>
+      <c r="J56" s="115"/>
+      <c r="K56" s="116"/>
+      <c r="L56" s="116"/>
+      <c r="M56" s="116"/>
+      <c r="N56" s="116"/>
+      <c r="O56" s="116"/>
+      <c r="P56" s="116"/>
+      <c r="Q56" s="116"/>
+      <c r="R56" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="106">
@@ -5964,13 +5920,11 @@
     <mergeCell ref="I20:I21"/>
     <mergeCell ref="G20:H20"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="87" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;C
-&amp;R&amp;G</oddHeader>
-    <oddFooter>&amp;L&amp;8
-OPRACOWAŁ: MARCIN DOMAGAŁA &amp;C&amp;8WERSJA DOKUMENTU 2, Z DNIA 2019-06-07&amp;R&amp;8OBOWIĄZUJE OD 2013-11-07</oddFooter>
+    <oddHeader>&amp;R&amp;G</oddHeader>
+    <oddFooter>&amp;L&amp;8OPRACOWAŁ: MARCIN DOMAGAŁA &amp;C&amp;8WERSJA DOKUMENTU 2, Z DNIA 2019-06-07&amp;R&amp;8OBOWIĄZUJE OD 2013-11-07</oddFooter>
   </headerFooter>
   <ignoredErrors>
     <ignoredError sqref="R25" numberStoredAsText="1"/>
@@ -5979,240 +5933,216 @@
   <legacyDrawing r:id="rId3"/>
   <legacyDrawingHF r:id="rId4"/>
   <oleObjects>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <oleObject progId="Equation.3" shapeId="1025" r:id="rId5">
-          <objectPr defaultSize="0" autoPict="0" r:id="rId6">
-            <anchor moveWithCells="1" sizeWithCells="1">
-              <from>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>114300</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>13</xdr:col>
-                <xdr:colOff>342900</xdr:colOff>
-                <xdr:row>26</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </objectPr>
-        </oleObject>
-      </mc:Choice>
-      <mc:Fallback>
-        <oleObject progId="Equation.3" shapeId="1025" r:id="rId5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
+    <oleObject progId="Equation.3" shapeId="1025" r:id="rId5"/>
   </oleObjects>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:Q9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="2" spans="2:17" ht="15" thickBot="1">
-      <c r="B2" s="134" t="s">
+    <row r="2" spans="2:17" ht="14.4" thickBot="1">
+      <c r="B2" s="146" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="134"/>
-      <c r="D2" s="134"/>
-      <c r="E2" s="135"/>
-      <c r="F2" s="125" t="s">
+      <c r="C2" s="146"/>
+      <c r="D2" s="146"/>
+      <c r="E2" s="147"/>
+      <c r="F2" s="139" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="134"/>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="134"/>
-      <c r="M2" s="134"/>
-      <c r="N2" s="134" t="s">
+      <c r="G2" s="146"/>
+      <c r="H2" s="146"/>
+      <c r="I2" s="146"/>
+      <c r="J2" s="146"/>
+      <c r="K2" s="146"/>
+      <c r="L2" s="146"/>
+      <c r="M2" s="146"/>
+      <c r="N2" s="146" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="134"/>
-      <c r="P2" s="134"/>
-      <c r="Q2" s="134"/>
+      <c r="O2" s="146"/>
+      <c r="P2" s="146"/>
+      <c r="Q2" s="146"/>
     </row>
     <row r="3" spans="2:17">
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="136"/>
-      <c r="F3" s="137" t="s">
+      <c r="C3" s="77"/>
+      <c r="D3" s="77"/>
+      <c r="E3" s="148"/>
+      <c r="F3" s="149" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="137" t="s">
+      <c r="G3" s="149"/>
+      <c r="H3" s="149"/>
+      <c r="I3" s="149"/>
+      <c r="J3" s="149" t="s">
         <v>56</v>
       </c>
-      <c r="K3" s="137"/>
-      <c r="L3" s="137"/>
-      <c r="M3" s="138"/>
-      <c r="N3" s="139"/>
-      <c r="O3" s="139"/>
-      <c r="P3" s="139"/>
-      <c r="Q3" s="139"/>
+      <c r="K3" s="149"/>
+      <c r="L3" s="149"/>
+      <c r="M3" s="150"/>
+      <c r="N3" s="151"/>
+      <c r="O3" s="151"/>
+      <c r="P3" s="151"/>
+      <c r="Q3" s="151"/>
     </row>
     <row r="4" spans="2:17">
-      <c r="B4" s="140" t="s">
+      <c r="B4" s="152" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="140"/>
-      <c r="D4" s="140"/>
-      <c r="E4" s="141"/>
-      <c r="F4" s="92" t="s">
+      <c r="C4" s="152"/>
+      <c r="D4" s="152"/>
+      <c r="E4" s="153"/>
+      <c r="F4" s="104" t="s">
         <v>49</v>
       </c>
-      <c r="G4" s="92"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="92"/>
-      <c r="J4" s="92" t="s">
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
+      <c r="J4" s="104" t="s">
         <v>57</v>
       </c>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="142"/>
-      <c r="O4" s="142"/>
-      <c r="P4" s="142"/>
-      <c r="Q4" s="142"/>
+      <c r="K4" s="104"/>
+      <c r="L4" s="104"/>
+      <c r="M4" s="107"/>
+      <c r="N4" s="154"/>
+      <c r="O4" s="154"/>
+      <c r="P4" s="154"/>
+      <c r="Q4" s="154"/>
     </row>
     <row r="5" spans="2:17">
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="152" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="140"/>
-      <c r="D5" s="140"/>
-      <c r="E5" s="141"/>
-      <c r="F5" s="92" t="s">
+      <c r="C5" s="152"/>
+      <c r="D5" s="152"/>
+      <c r="E5" s="153"/>
+      <c r="F5" s="104" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="92"/>
-      <c r="H5" s="92"/>
-      <c r="I5" s="92"/>
-      <c r="J5" s="92" t="s">
+      <c r="G5" s="104"/>
+      <c r="H5" s="104"/>
+      <c r="I5" s="104"/>
+      <c r="J5" s="104" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="92"/>
-      <c r="L5" s="92"/>
-      <c r="M5" s="95"/>
-      <c r="N5" s="142"/>
-      <c r="O5" s="142"/>
-      <c r="P5" s="142"/>
-      <c r="Q5" s="142"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="104"/>
+      <c r="M5" s="107"/>
+      <c r="N5" s="154"/>
+      <c r="O5" s="154"/>
+      <c r="P5" s="154"/>
+      <c r="Q5" s="154"/>
     </row>
     <row r="6" spans="2:17">
-      <c r="B6" s="140" t="s">
+      <c r="B6" s="152" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="140"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="141"/>
-      <c r="F6" s="92" t="s">
+      <c r="C6" s="152"/>
+      <c r="D6" s="152"/>
+      <c r="E6" s="153"/>
+      <c r="F6" s="104" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="93" t="s">
+      <c r="G6" s="104"/>
+      <c r="H6" s="104"/>
+      <c r="I6" s="107"/>
+      <c r="J6" s="105" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="92"/>
-      <c r="L6" s="92"/>
-      <c r="M6" s="95"/>
-      <c r="N6" s="142"/>
-      <c r="O6" s="142"/>
-      <c r="P6" s="142"/>
-      <c r="Q6" s="142"/>
+      <c r="K6" s="104"/>
+      <c r="L6" s="104"/>
+      <c r="M6" s="107"/>
+      <c r="N6" s="154"/>
+      <c r="O6" s="154"/>
+      <c r="P6" s="154"/>
+      <c r="Q6" s="154"/>
     </row>
     <row r="7" spans="2:17">
-      <c r="B7" s="140" t="s">
+      <c r="B7" s="152" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="140"/>
-      <c r="D7" s="140"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="92" t="s">
+      <c r="C7" s="152"/>
+      <c r="D7" s="152"/>
+      <c r="E7" s="153"/>
+      <c r="F7" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="92"/>
-      <c r="H7" s="92"/>
-      <c r="I7" s="95"/>
-      <c r="J7" s="93" t="s">
+      <c r="G7" s="104"/>
+      <c r="H7" s="104"/>
+      <c r="I7" s="107"/>
+      <c r="J7" s="105" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92"/>
-      <c r="M7" s="95"/>
-      <c r="N7" s="142"/>
-      <c r="O7" s="142"/>
-      <c r="P7" s="142"/>
-      <c r="Q7" s="142"/>
+      <c r="K7" s="104"/>
+      <c r="L7" s="104"/>
+      <c r="M7" s="107"/>
+      <c r="N7" s="154"/>
+      <c r="O7" s="154"/>
+      <c r="P7" s="154"/>
+      <c r="Q7" s="154"/>
     </row>
     <row r="8" spans="2:17">
-      <c r="B8" s="140" t="s">
+      <c r="B8" s="152" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="140"/>
-      <c r="D8" s="140"/>
-      <c r="E8" s="141"/>
-      <c r="F8" s="92" t="s">
+      <c r="C8" s="152"/>
+      <c r="D8" s="152"/>
+      <c r="E8" s="153"/>
+      <c r="F8" s="104" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92" t="s">
+      <c r="G8" s="104"/>
+      <c r="H8" s="104"/>
+      <c r="I8" s="104"/>
+      <c r="J8" s="104" t="s">
         <v>61</v>
       </c>
-      <c r="K8" s="92"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="95"/>
-      <c r="N8" s="142"/>
-      <c r="O8" s="142"/>
-      <c r="P8" s="142"/>
-      <c r="Q8" s="142"/>
+      <c r="K8" s="104"/>
+      <c r="L8" s="104"/>
+      <c r="M8" s="107"/>
+      <c r="N8" s="154"/>
+      <c r="O8" s="154"/>
+      <c r="P8" s="154"/>
+      <c r="Q8" s="154"/>
     </row>
     <row r="9" spans="2:17">
-      <c r="B9" s="140" t="s">
+      <c r="B9" s="152" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="140"/>
-      <c r="D9" s="140"/>
-      <c r="E9" s="141"/>
-      <c r="F9" s="92" t="s">
+      <c r="C9" s="152"/>
+      <c r="D9" s="152"/>
+      <c r="E9" s="153"/>
+      <c r="F9" s="104" t="s">
         <v>54</v>
       </c>
-      <c r="G9" s="92"/>
-      <c r="H9" s="92" t="s">
+      <c r="G9" s="104"/>
+      <c r="H9" s="104" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="95"/>
-      <c r="J9" s="93" t="s">
+      <c r="I9" s="107"/>
+      <c r="J9" s="105" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="92"/>
-      <c r="L9" s="92">
+      <c r="K9" s="104"/>
+      <c r="L9" s="104">
         <v>2.5</v>
       </c>
-      <c r="M9" s="95"/>
-      <c r="N9" s="142"/>
-      <c r="O9" s="142"/>
-      <c r="P9" s="142"/>
-      <c r="Q9" s="142"/>
+      <c r="M9" s="107"/>
+      <c r="N9" s="154"/>
+      <c r="O9" s="154"/>
+      <c r="P9" s="154"/>
+      <c r="Q9" s="154"/>
     </row>
   </sheetData>
   <mergeCells count="33">

</xml_diff>